<commit_message>
Add testing methodology and standards compliance documentation
Co-authored-by: yalovali <234063+yalovali@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/__PROJECT_BACKLOG.xlsx
+++ b/docs/__PROJECT_BACKLOG.xlsx
@@ -1295,12 +1295,12 @@
       </c>
       <c r="F14" s="18" t="inlineStr">
         <is>
-          <t>Playwright tests exist (no entity management)</t>
+          <t>CTestCase, CTestScenario, CTestRun, CTestStep, CTestCaseType, CTestCaseResult, CTestStepResult</t>
         </is>
       </c>
       <c r="G14" s="18" t="inlineStr">
         <is>
-          <t>testcases (missing)</t>
+          <t>tech.derbent.app.testcases</t>
         </is>
       </c>
       <c r="H14" s="18" t="n">
@@ -2189,7 +2189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
@@ -3866,11 +3866,256 @@
         <v/>
       </c>
     </row>
-    <row r="33" ht="13.5" customHeight="1" s="15"/>
-    <row r="34" ht="13.5" customHeight="1" s="15"/>
-    <row r="35" ht="13.5" customHeight="1" s="15"/>
-    <row r="36" ht="13.5" customHeight="1" s="15"/>
-    <row r="37" ht="13.5" customHeight="1" s="15"/>
+    <row r="33" ht="13.5" customHeight="1" s="15">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Test Case Management</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Create, read, update, delete test cases with full workflow support, test steps, and metadata</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Users can create test cases with steps, assign types, set priority/severity, link to scenarios, view history</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Views for CTestCase and CTestStep, grid with filtering, dialog forms, test step inline editor</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>CTestCase, CTestStep, CTestCaseView, CTestCaseService</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>8</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="13.5" customHeight="1" s="15">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Test Scenario Management</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Organize test cases into scenarios representing business workflows or features</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Users can create scenarios, add test cases to scenarios, view scenario coverage, manage scenario lifecycle</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>CTestScenarioView with grid and dialog, link to test cases, scenario execution planning</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>CTestScenario, CTestScenarioView, CTestScenarioService</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>5</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="13.5" customHeight="1" s="15">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Test Execution &amp; Results</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Execute test runs, record step-by-step results, track pass/fail metrics</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Users can create test runs from scenarios, execute tests step-by-step, record actual results, attach evidence, view statistics</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>CTestRunView with execution workflow, result recording dialogs, progress tracking, metrics dashboard</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>CTestRun, CTestCaseResult, CTestStepResult, CTestRunView, CTestRunService</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>13</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="13.5" customHeight="1" s="15">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>F13.4</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Test Type Configuration</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Configure test case types with workflows and statuses</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Admins can create test case types, assign workflows, configure colors/icons, manage type lifecycle</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>CTestCaseTypeView (admin), type initializer service, workflow integration</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>CTestCaseType, CTestCaseTypeView, CTestCaseTypeInitializerService</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>3</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="13.5" customHeight="1" s="15">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Test Reporting &amp; Analytics</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Dashboard and reports for test metrics, coverage, trends</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Users can view test metrics dashboard, analyze pass/fail trends, review test coverage by feature, export reports</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Dashboard component, metrics calculation, chart widgets, report generation</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>CComponentTestMetrics, CTestReportService, dashboard integration</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>8</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
     <row r="38" ht="13.5" customHeight="1" s="15"/>
     <row r="39" ht="13.5" customHeight="1" s="15"/>
     <row r="40" ht="13.5" customHeight="1" s="15"/>
@@ -3897,7 +4142,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
@@ -5744,6 +5989,686 @@
       </c>
       <c r="F48" s="14" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to create test cases with detailed steps so that I can document test procedures</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Can create test case with name, description, preconditions; Can add ordered test steps with action and expected result; Can save and view created test case</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Use CEntityFormBuilder for test case form, embed test step grid with inline editing, validate required fields</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>3</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>US13.1.2</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to assign priority and severity to test cases so that I can prioritize testing</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Can select priority (LOW/MEDIUM/HIGH/CRITICAL); Can select severity (TRIVIAL/MINOR/NORMAL/MAJOR/BLOCKER); Values are saved and displayed in grid</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Use enum fields with dropdown, display with colored badges in grid</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>US13.1.3</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to mark test cases as automated and link to test code so that I can integrate manual and automated testing</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Can toggle automated flag; Can enter automated test path; Automated tests are visually distinguished in grid</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Checkbox for automated flag, text field for path, grid column renderer with icon</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>2</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>US13.1.4</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to view and filter test cases so that I can find relevant tests</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Can view all test cases in grid; Can filter by type, priority, severity, automated; Can search by name/description; Can sort by columns</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Use CGrid with standard filter toolbar, implement filter providers for enums</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>US13.2.1</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to create test scenarios to group related test cases</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Can create scenario with name, description, objective; Can save and view scenarios in grid</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Use standard view pattern with CGrid and dialog form</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>US13.2.2</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to add test cases to scenarios so that I can organize tests by feature</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Can link test case to scenario via dropdown/selector; Can view test cases grouped by scenario; Can remove test case from scenario</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Implement entity selector in test case form, add scenario filter to test case grid</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>2</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>US13.2.3</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to view scenario completion status so that I can track testing progress</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Can see count of total/passed/failed test cases in scenario; Can view pass rate percentage; Status updates automatically</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Add calculated fields to scenario entity, display in grid and detail view</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>US13.3.1</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to create a test run from a scenario so that I can execute a group of tests</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Can select scenario and create test run; Test run is initialized with all test cases from scenario; Can enter environment and build number</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Create test run dialog with scenario selector, auto-populate test cases, initialize result entities</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>3</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>US13.3.2</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to execute test cases step-by-step and record results</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Can view test case steps in execution view; Can mark each step as PASSED/FAILED/BLOCKED/SKIPPED; Can enter actual results; Can proceed to next test case</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Create test execution component with step navigator, result recorder, progress tracker</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>5</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>US13.3.3</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to attach screenshots and logs to test results</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Can upload attachments during execution; Can attach files to test run or specific test case result; Attachments are linked and accessible</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Reuse existing attachment component, link to test run and test case result entities</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>2</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>US13.3.4</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to view test run statistics so that I can assess quality</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Can view total/passed/failed counts for test cases and steps; Can see pass rate percentage; Can view execution duration; Statistics update in real-time</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Calculate and display metrics in test run view, add summary panel</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>2</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>US13.3.5</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to complete a test run and view results history</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Can mark test run as complete; Can view list of all test runs; Can reopen completed test runs for review; Can compare results across runs</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Add complete button, implement test run history grid, enable result comparison view</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>US13.4.1</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>F13.4</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>As an admin, I want to configure test case types so that I can categorize tests</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Can create test case type with name, color, icon; Can assign workflow to type; Types appear in test case type dropdown</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Create admin view for test case types, reuse type entity patterns</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>2</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>US13.4.2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>F13.4</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>As an admin, I want to define workflows for test case types</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Can select workflow for each type; Test cases follow assigned workflow statuses; Workflow rules apply to test cases of that type</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Workflow assignment in type entity, enforce workflow in test case service</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>US13.5.1</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>As a project manager, I want to view a test metrics dashboard</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Can view overall test coverage metrics; Can see pass/fail trends over time; Can drill down into failed tests</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Create dashboard component with charts and metrics, integrate with project dashboard</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>3</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>US13.5.2</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>As a project manager, I want to export test reports</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Can generate test summary report; Can export to PDF or Excel; Report includes all test run details and statistics</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Implement report generation service, add export buttons to test run view</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>3</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>US13.5.3</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>As a QA engineer, I want to see test coverage by feature</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Can view which features have test coverage; Can identify gaps in test coverage; Coverage percentage is calculated automatically</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Link test scenarios to features, calculate coverage metrics, display coverage matrix</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>2</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -14305,1520 +15230,1520 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" t="inlineStr">
+      <c r="A213" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B213" t="inlineStr">
+      <c r="B213" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C213" t="inlineStr">
+      <c r="C213" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D213" t="inlineStr">
+      <c r="D213" s="14" t="inlineStr">
         <is>
           <t>Create CTestScenario entity (groups of test cases)</t>
         </is>
       </c>
-      <c r="E213" t="n">
+      <c r="E213" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F213" t="inlineStr">
+      <c r="F213" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G213" t="inlineStr">
+      <c r="G213" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testscenario.domain.CTestScenario</t>
         </is>
       </c>
-      <c r="H213" t="inlineStr">
+      <c r="H213" s="14" t="inlineStr">
         <is>
           <t>Extend CEntityOfProject, has test cases, comments, attachments</t>
         </is>
       </c>
     </row>
     <row r="214">
-      <c r="A214" t="inlineStr">
+      <c r="A214" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B214" t="inlineStr">
+      <c r="B214" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C214" t="inlineStr">
+      <c r="C214" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D214" t="inlineStr">
+      <c r="D214" s="14" t="inlineStr">
         <is>
           <t>Create CTestStep entity (individual test steps)</t>
         </is>
       </c>
-      <c r="E214" t="n">
+      <c r="E214" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F214" t="inlineStr">
+      <c r="F214" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G214" t="inlineStr">
+      <c r="G214" s="14" t="inlineStr">
         <is>
           <t>app.testcases.teststep.domain.CTestStep</t>
         </is>
       </c>
-      <c r="H214" t="inlineStr">
+      <c r="H214" s="14" t="inlineStr">
         <is>
           <t>Step order, action, expected result, test data</t>
         </is>
       </c>
     </row>
     <row r="215">
-      <c r="A215" t="inlineStr">
+      <c r="A215" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B215" t="inlineStr">
+      <c r="B215" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C215" t="inlineStr">
+      <c r="C215" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D215" t="inlineStr">
+      <c r="D215" s="14" t="inlineStr">
         <is>
           <t>Create CTestCase entity with steps</t>
         </is>
       </c>
-      <c r="E215" t="n">
+      <c r="E215" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F215" t="inlineStr">
+      <c r="F215" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G215" t="inlineStr">
+      <c r="G215" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testcase.domain.CTestCase</t>
         </is>
       </c>
-      <c r="H215" t="inlineStr">
+      <c r="H215" s="14" t="inlineStr">
         <is>
           <t>Extend CProjectItem, has test steps, comments, attachments, workflow</t>
         </is>
       </c>
     </row>
     <row r="216">
-      <c r="A216" t="inlineStr">
+      <c r="A216" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B216" t="inlineStr">
+      <c r="B216" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C216" t="inlineStr">
+      <c r="C216" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D216" t="inlineStr">
+      <c r="D216" s="14" t="inlineStr">
         <is>
           <t>Create CTestCaseType entity</t>
         </is>
       </c>
-      <c r="E216" t="n">
+      <c r="E216" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F216" t="inlineStr">
+      <c r="F216" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G216" t="inlineStr">
+      <c r="G216" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testcasetype.domain.CTestCaseType</t>
         </is>
       </c>
-      <c r="H216" t="inlineStr">
+      <c r="H216" s="14" t="inlineStr">
         <is>
           <t>Extend CTypeEntity for test categorization</t>
         </is>
       </c>
     </row>
     <row r="217">
-      <c r="A217" t="inlineStr">
+      <c r="A217" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B217" t="inlineStr">
+      <c r="B217" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
+      <c r="C217" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D217" t="inlineStr">
+      <c r="D217" s="14" t="inlineStr">
         <is>
           <t>Create CTestResult enum</t>
         </is>
       </c>
-      <c r="E217" t="n">
+      <c r="E217" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F217" t="inlineStr">
+      <c r="F217" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G217" t="inlineStr">
+      <c r="G217" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testexecution.domain.CTestResult</t>
         </is>
       </c>
-      <c r="H217" t="inlineStr">
+      <c r="H217" s="14" t="inlineStr">
         <is>
           <t>PASSED/FAILED/BLOCKED/SKIPPED/IN_PROGRESS/NOT_EXECUTED</t>
         </is>
       </c>
     </row>
     <row r="218">
-      <c r="A218" t="inlineStr">
+      <c r="A218" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B218" t="inlineStr">
+      <c r="B218" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C218" t="inlineStr">
+      <c r="C218" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D218" t="inlineStr">
+      <c r="D218" s="14" t="inlineStr">
         <is>
           <t>Create CTestExecution entity</t>
         </is>
       </c>
-      <c r="E218" t="n">
+      <c r="E218" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F218" t="inlineStr">
+      <c r="F218" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G218" t="inlineStr">
+      <c r="G218" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testexecution.domain.CTestExecution</t>
         </is>
       </c>
-      <c r="H218" t="inlineStr">
+      <c r="H218" s="14" t="inlineStr">
         <is>
           <t>Track test runs, results, duration, errors</t>
         </is>
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="inlineStr">
+      <c r="A219" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B219" t="inlineStr">
+      <c r="B219" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C219" t="inlineStr">
+      <c r="C219" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D219" t="inlineStr">
+      <c r="D219" s="14" t="inlineStr">
         <is>
           <t>Create CTestPriority enum</t>
         </is>
       </c>
-      <c r="E219" t="n">
+      <c r="E219" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F219" t="inlineStr">
+      <c r="F219" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G219" t="inlineStr">
+      <c r="G219" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testcase.domain.CTestPriority</t>
         </is>
       </c>
-      <c r="H219" t="inlineStr">
+      <c r="H219" s="14" t="inlineStr">
         <is>
           <t>CRITICAL/HIGH/MEDIUM/LOW</t>
         </is>
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="inlineStr">
+      <c r="A220" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B220" t="inlineStr">
+      <c r="B220" s="14" t="inlineStr">
         <is>
           <t>Test Management Entities</t>
         </is>
       </c>
-      <c r="C220" t="inlineStr">
+      <c r="C220" s="14" t="inlineStr">
         <is>
           <t>As a QA, I need test management structure</t>
         </is>
       </c>
-      <c r="D220" t="inlineStr">
+      <c r="D220" s="14" t="inlineStr">
         <is>
           <t>Create CTestSeverity enum</t>
         </is>
       </c>
-      <c r="E220" t="n">
+      <c r="E220" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F220" t="inlineStr">
+      <c r="F220" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G220" t="inlineStr">
+      <c r="G220" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testcase.domain.CTestSeverity</t>
         </is>
       </c>
-      <c r="H220" t="inlineStr">
+      <c r="H220" s="14" t="inlineStr">
         <is>
           <t>BLOCKER/CRITICAL/MAJOR/NORMAL/MINOR/TRIVIAL</t>
         </is>
       </c>
     </row>
     <row r="221">
-      <c r="A221" t="inlineStr">
+      <c r="A221" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B221" t="inlineStr">
+      <c r="B221" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C221" t="inlineStr">
+      <c r="C221" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D221" t="inlineStr">
+      <c r="D221" s="14" t="inlineStr">
         <is>
           <t>Create ITestScenarioRepository</t>
         </is>
       </c>
-      <c r="E221" t="n">
+      <c r="E221" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F221" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G221" t="inlineStr">
+      <c r="F221" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G221" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testscenario.service</t>
         </is>
       </c>
-      <c r="H221" t="inlineStr">
+      <c r="H221" s="14" t="inlineStr">
         <is>
           <t>Repository with proper ordering</t>
         </is>
       </c>
     </row>
     <row r="222">
-      <c r="A222" t="inlineStr">
+      <c r="A222" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B222" t="inlineStr">
+      <c r="B222" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C222" t="inlineStr">
+      <c r="C222" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D222" t="inlineStr">
+      <c r="D222" s="14" t="inlineStr">
         <is>
           <t>Create CTestScenarioService</t>
         </is>
       </c>
-      <c r="E222" t="n">
+      <c r="E222" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F222" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G222" t="inlineStr">
+      <c r="F222" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G222" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testscenario.service</t>
         </is>
       </c>
-      <c r="H222" t="inlineStr">
+      <c r="H222" s="14" t="inlineStr">
         <is>
           <t>CRUD and validation logic</t>
         </is>
       </c>
     </row>
     <row r="223">
-      <c r="A223" t="inlineStr">
+      <c r="A223" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B223" t="inlineStr">
+      <c r="B223" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C223" t="inlineStr">
+      <c r="C223" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D223" t="inlineStr">
+      <c r="D223" s="14" t="inlineStr">
         <is>
           <t>Create ITestCaseRepository</t>
         </is>
       </c>
-      <c r="E223" t="n">
+      <c r="E223" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F223" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G223" t="inlineStr">
+      <c r="F223" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G223" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testcase.service</t>
         </is>
       </c>
-      <c r="H223" t="inlineStr">
+      <c r="H223" s="14" t="inlineStr">
         <is>
           <t>Repository with proper ordering</t>
         </is>
       </c>
     </row>
     <row r="224">
-      <c r="A224" t="inlineStr">
+      <c r="A224" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B224" t="inlineStr">
+      <c r="B224" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C224" t="inlineStr">
+      <c r="C224" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D224" t="inlineStr">
+      <c r="D224" s="14" t="inlineStr">
         <is>
           <t>Create CTestCaseService</t>
         </is>
       </c>
-      <c r="E224" t="n">
+      <c r="E224" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F224" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G224" t="inlineStr">
+      <c r="F224" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G224" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testcase.service</t>
         </is>
       </c>
-      <c r="H224" t="inlineStr">
+      <c r="H224" s="14" t="inlineStr">
         <is>
           <t>CRUD and validation logic</t>
         </is>
       </c>
     </row>
     <row r="225">
-      <c r="A225" t="inlineStr">
+      <c r="A225" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B225" t="inlineStr">
+      <c r="B225" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C225" t="inlineStr">
+      <c r="C225" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D225" t="inlineStr">
+      <c r="D225" s="14" t="inlineStr">
         <is>
           <t>Create ITestStepRepository</t>
         </is>
       </c>
-      <c r="E225" t="n">
+      <c r="E225" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F225" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G225" t="inlineStr">
+      <c r="F225" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G225" s="14" t="inlineStr">
         <is>
           <t>app.testcases.teststep.service</t>
         </is>
       </c>
-      <c r="H225" t="inlineStr">
+      <c r="H225" s="14" t="inlineStr">
         <is>
           <t>Repository with step ordering</t>
         </is>
       </c>
     </row>
     <row r="226">
-      <c r="A226" t="inlineStr">
+      <c r="A226" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B226" t="inlineStr">
+      <c r="B226" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C226" t="inlineStr">
+      <c r="C226" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D226" t="inlineStr">
+      <c r="D226" s="14" t="inlineStr">
         <is>
           <t>Create CTestStepService</t>
         </is>
       </c>
-      <c r="E226" t="n">
+      <c r="E226" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F226" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G226" t="inlineStr">
+      <c r="F226" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G226" s="14" t="inlineStr">
         <is>
           <t>app.testcases.teststep.service</t>
         </is>
       </c>
-      <c r="H226" t="inlineStr">
+      <c r="H226" s="14" t="inlineStr">
         <is>
           <t>CRUD, reordering steps</t>
         </is>
       </c>
     </row>
     <row r="227">
-      <c r="A227" t="inlineStr">
+      <c r="A227" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B227" t="inlineStr">
+      <c r="B227" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C227" t="inlineStr">
+      <c r="C227" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D227" t="inlineStr">
+      <c r="D227" s="14" t="inlineStr">
         <is>
           <t>Create ITestExecutionRepository</t>
         </is>
       </c>
-      <c r="E227" t="n">
+      <c r="E227" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F227" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G227" t="inlineStr">
+      <c r="F227" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G227" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testexecution.service</t>
         </is>
       </c>
-      <c r="H227" t="inlineStr">
+      <c r="H227" s="14" t="inlineStr">
         <is>
           <t>Repository with execution tracking</t>
         </is>
       </c>
     </row>
     <row r="228">
-      <c r="A228" t="inlineStr">
+      <c r="A228" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B228" t="inlineStr">
+      <c r="B228" s="14" t="inlineStr">
         <is>
           <t>Test Management Services</t>
         </is>
       </c>
-      <c r="C228" t="inlineStr">
+      <c r="C228" s="14" t="inlineStr">
         <is>
           <t>As a developer, I need test services</t>
         </is>
       </c>
-      <c r="D228" t="inlineStr">
+      <c r="D228" s="14" t="inlineStr">
         <is>
           <t>Create CTestExecutionService</t>
         </is>
       </c>
-      <c r="E228" t="n">
+      <c r="E228" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F228" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G228" t="inlineStr">
+      <c r="F228" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G228" s="14" t="inlineStr">
         <is>
           <t>app.testcases.testexecution.service</t>
         </is>
       </c>
-      <c r="H228" t="inlineStr">
+      <c r="H228" s="14" t="inlineStr">
         <is>
           <t>Track execution history, results</t>
         </is>
       </c>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr">
+      <c r="A229" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B229" t="inlineStr">
+      <c r="B229" s="14" t="inlineStr">
         <is>
           <t>Test Management UI</t>
         </is>
       </c>
-      <c r="C229" t="inlineStr">
+      <c r="C229" s="14" t="inlineStr">
         <is>
           <t>As a QA, I want test management views</t>
         </is>
       </c>
-      <c r="D229" t="inlineStr">
+      <c r="D229" s="14" t="inlineStr">
         <is>
           <t>Create Test Scenarios view</t>
         </is>
       </c>
-      <c r="E229" t="n">
+      <c r="E229" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F229" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G229" t="inlineStr">
+      <c r="F229" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G229" s="14" t="inlineStr">
         <is>
           <t>app.testcases.view.CPageTestScenario</t>
         </is>
       </c>
-      <c r="H229" t="inlineStr">
+      <c r="H229" s="14" t="inlineStr">
         <is>
           <t>Grid with CRUD, filtering by project</t>
         </is>
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr">
+      <c r="A230" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B230" t="inlineStr">
+      <c r="B230" s="14" t="inlineStr">
         <is>
           <t>Test Management UI</t>
         </is>
       </c>
-      <c r="C230" t="inlineStr">
+      <c r="C230" s="14" t="inlineStr">
         <is>
           <t>As a QA, I want test management views</t>
         </is>
       </c>
-      <c r="D230" t="inlineStr">
+      <c r="D230" s="14" t="inlineStr">
         <is>
           <t>Create Test Cases view</t>
         </is>
       </c>
-      <c r="E230" t="n">
+      <c r="E230" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F230" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G230" t="inlineStr">
+      <c r="F230" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G230" s="14" t="inlineStr">
         <is>
           <t>app.testcases.view.CPageTestCase</t>
         </is>
       </c>
-      <c r="H230" t="inlineStr">
+      <c r="H230" s="14" t="inlineStr">
         <is>
           <t>Grid with CRUD, test step management</t>
         </is>
       </c>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr">
+      <c r="A231" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B231" t="inlineStr">
+      <c r="B231" s="14" t="inlineStr">
         <is>
           <t>Test Management UI</t>
         </is>
       </c>
-      <c r="C231" t="inlineStr">
+      <c r="C231" s="14" t="inlineStr">
         <is>
           <t>As a QA, I want test management views</t>
         </is>
       </c>
-      <c r="D231" t="inlineStr">
+      <c r="D231" s="14" t="inlineStr">
         <is>
           <t>Create Test Steps management dialog</t>
         </is>
       </c>
-      <c r="E231" t="n">
+      <c r="E231" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F231" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G231" t="inlineStr">
+      <c r="F231" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G231" s="14" t="inlineStr">
         <is>
           <t>app.testcases.view.CDialogTestSteps</t>
         </is>
       </c>
-      <c r="H231" t="inlineStr">
+      <c r="H231" s="14" t="inlineStr">
         <is>
           <t>Ordered list with drag-drop reordering</t>
         </is>
       </c>
     </row>
     <row r="232">
-      <c r="A232" t="inlineStr">
+      <c r="A232" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B232" t="inlineStr">
+      <c r="B232" s="14" t="inlineStr">
         <is>
           <t>Test Management UI</t>
         </is>
       </c>
-      <c r="C232" t="inlineStr">
+      <c r="C232" s="14" t="inlineStr">
         <is>
           <t>As a QA, I want test management views</t>
         </is>
       </c>
-      <c r="D232" t="inlineStr">
+      <c r="D232" s="14" t="inlineStr">
         <is>
           <t>Create Test Execution tracking view</t>
         </is>
       </c>
-      <c r="E232" t="n">
+      <c r="E232" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F232" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G232" t="inlineStr">
+      <c r="F232" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G232" s="14" t="inlineStr">
         <is>
           <t>app.testcases.view.CPageTestExecution</t>
         </is>
       </c>
-      <c r="H232" t="inlineStr">
+      <c r="H232" s="14" t="inlineStr">
         <is>
           <t>Execute tests, record results</t>
         </is>
       </c>
     </row>
     <row r="233">
-      <c r="A233" t="inlineStr">
+      <c r="A233" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
+      <c r="B233" s="14" t="inlineStr">
         <is>
           <t>Test Management UI</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr">
+      <c r="C233" s="14" t="inlineStr">
         <is>
           <t>As a QA, I want test management views</t>
         </is>
       </c>
-      <c r="D233" t="inlineStr">
+      <c r="D233" s="14" t="inlineStr">
         <is>
           <t>Create Test Coverage dashboard</t>
         </is>
       </c>
-      <c r="E233" t="n">
+      <c r="E233" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F233" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G233" t="inlineStr">
+      <c r="F233" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G233" s="14" t="inlineStr">
         <is>
           <t>app.testcases.view.CTestCoverageDashboard</t>
         </is>
       </c>
-      <c r="H233" t="inlineStr">
+      <c r="H233" s="14" t="inlineStr">
         <is>
           <t>Coverage charts, pass/fail rates</t>
         </is>
       </c>
     </row>
     <row r="234">
-      <c r="A234" t="inlineStr">
+      <c r="A234" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B234" t="inlineStr">
+      <c r="B234" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Integration</t>
         </is>
       </c>
-      <c r="C234" t="inlineStr">
+      <c r="C234" s="14" t="inlineStr">
         <is>
           <t>As a developer, I want Playwright integration</t>
         </is>
       </c>
-      <c r="D234" t="inlineStr">
+      <c r="D234" s="14" t="inlineStr">
         <is>
           <t>Link Playwright tests to test cases</t>
         </is>
       </c>
-      <c r="E234" t="n">
+      <c r="E234" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F234" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G234" t="inlineStr">
+      <c r="F234" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G234" s="14" t="inlineStr">
         <is>
           <t>app.testcases.service integration</t>
         </is>
       </c>
-      <c r="H234" t="inlineStr">
+      <c r="H234" s="14" t="inlineStr">
         <is>
           <t>Map automated tests to entities by test path</t>
         </is>
       </c>
     </row>
     <row r="235">
-      <c r="A235" t="inlineStr">
+      <c r="A235" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B235" t="inlineStr">
+      <c r="B235" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Integration</t>
         </is>
       </c>
-      <c r="C235" t="inlineStr">
+      <c r="C235" s="14" t="inlineStr">
         <is>
           <t>As a developer, I want Playwright integration</t>
         </is>
       </c>
-      <c r="D235" t="inlineStr">
+      <c r="D235" s="14" t="inlineStr">
         <is>
           <t>Auto-import Playwright test results</t>
         </is>
       </c>
-      <c r="E235" t="n">
+      <c r="E235" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F235" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G235" t="inlineStr">
+      <c r="F235" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G235" s="14" t="inlineStr">
         <is>
           <t>app.testcases.service.CTestImportService</t>
         </is>
       </c>
-      <c r="H235" t="inlineStr">
+      <c r="H235" s="14" t="inlineStr">
         <is>
           <t>Parse test output, create executions</t>
         </is>
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr">
+      <c r="A236" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B236" t="inlineStr">
+      <c r="B236" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Integration</t>
         </is>
       </c>
-      <c r="C236" t="inlineStr">
+      <c r="C236" s="14" t="inlineStr">
         <is>
           <t>As a developer, I want Playwright integration</t>
         </is>
       </c>
-      <c r="D236" t="inlineStr">
+      <c r="D236" s="14" t="inlineStr">
         <is>
           <t>Generate test cases from Playwright</t>
         </is>
       </c>
-      <c r="E236" t="n">
+      <c r="E236" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F236" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G236" t="inlineStr">
+      <c r="F236" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G236" s="14" t="inlineStr">
         <is>
           <t>app.testcases.service.CTestGeneratorService</t>
         </is>
       </c>
-      <c r="H236" t="inlineStr">
+      <c r="H236" s="14" t="inlineStr">
         <is>
           <t>Scan test files, auto-create test cases</t>
         </is>
       </c>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr">
+      <c r="A237" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B237" t="inlineStr">
+      <c r="B237" s="14" t="inlineStr">
         <is>
           <t>Test-Friendly Code Guidelines</t>
         </is>
       </c>
-      <c r="C237" t="inlineStr">
+      <c r="C237" s="14" t="inlineStr">
         <is>
           <t>As a developer, I follow test-friendly patterns</t>
         </is>
       </c>
-      <c r="D237" t="inlineStr">
+      <c r="D237" s="14" t="inlineStr">
         <is>
           <t>Enforce component ID generation via CAuxillaries.setId</t>
         </is>
       </c>
-      <c r="E237" t="n">
+      <c r="E237" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F237" t="inlineStr">
+      <c r="F237" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G237" t="inlineStr">
+      <c r="G237" s="14" t="inlineStr">
         <is>
           <t>api.utils.CAuxillaries</t>
         </is>
       </c>
-      <c r="H237" t="inlineStr">
+      <c r="H237" s="14" t="inlineStr">
         <is>
           <t>All components auto-get IDs for test selectors</t>
         </is>
       </c>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr">
+      <c r="A238" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B238" t="inlineStr">
+      <c r="B238" s="14" t="inlineStr">
         <is>
           <t>Test-Friendly Code Guidelines</t>
         </is>
       </c>
-      <c r="C238" t="inlineStr">
+      <c r="C238" s="14" t="inlineStr">
         <is>
           <t>As a developer, I follow test-friendly patterns</t>
         </is>
       </c>
-      <c r="D238" t="inlineStr">
+      <c r="D238" s="14" t="inlineStr">
         <is>
           <t>Use consistent button IDs (cbutton-new, cbutton-save, etc)</t>
         </is>
       </c>
-      <c r="E238" t="n">
+      <c r="E238" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F238" t="inlineStr">
+      <c r="F238" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G238" t="inlineStr">
+      <c r="G238" s="14" t="inlineStr">
         <is>
           <t>api.ui.component.basic.CButton</t>
         </is>
       </c>
-      <c r="H238" t="inlineStr">
+      <c r="H238" s="14" t="inlineStr">
         <is>
           <t>Standardized CRUD button IDs</t>
         </is>
       </c>
     </row>
     <row r="239">
-      <c r="A239" t="inlineStr">
+      <c r="A239" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B239" t="inlineStr">
+      <c r="B239" s="14" t="inlineStr">
         <is>
           <t>Test-Friendly Code Guidelines</t>
         </is>
       </c>
-      <c r="C239" t="inlineStr">
+      <c r="C239" s="14" t="inlineStr">
         <is>
           <t>As a developer, I follow test-friendly patterns</t>
         </is>
       </c>
-      <c r="D239" t="inlineStr">
+      <c r="D239" s="14" t="inlineStr">
         <is>
           <t>Use field ID prefix pattern (field-xxx)</t>
         </is>
       </c>
-      <c r="E239" t="n">
+      <c r="E239" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F239" t="inlineStr">
+      <c r="F239" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G239" t="inlineStr">
+      <c r="G239" s="14" t="inlineStr">
         <is>
           <t>Various form fields</t>
         </is>
       </c>
-      <c r="H239" t="inlineStr">
+      <c r="H239" s="14" t="inlineStr">
         <is>
           <t>All form fields get predictable IDs</t>
         </is>
       </c>
     </row>
     <row r="240">
-      <c r="A240" t="inlineStr">
+      <c r="A240" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B240" t="inlineStr">
+      <c r="B240" s="14" t="inlineStr">
         <is>
           <t>Test-Friendly Code Guidelines</t>
         </is>
       </c>
-      <c r="C240" t="inlineStr">
+      <c r="C240" s="14" t="inlineStr">
         <is>
           <t>As a developer, I follow test-friendly patterns</t>
         </is>
       </c>
-      <c r="D240" t="inlineStr">
+      <c r="D240" s="14" t="inlineStr">
         <is>
           <t>Document ID selector patterns in tests</t>
         </is>
       </c>
-      <c r="E240" t="n">
+      <c r="E240" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F240" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G240" t="inlineStr">
+      <c r="F240" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G240" s="14" t="inlineStr">
         <is>
           <t>docs/testing/ID_SELECTOR_PATTERNS.md</t>
         </is>
       </c>
-      <c r="H240" t="inlineStr">
+      <c r="H240" s="14" t="inlineStr">
         <is>
           <t>Complete guide for test selectors</t>
         </is>
       </c>
     </row>
     <row r="241">
-      <c r="A241" t="inlineStr">
+      <c r="A241" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B241" t="inlineStr">
+      <c r="B241" s="14" t="inlineStr">
         <is>
           <t>Test-Friendly Code Guidelines</t>
         </is>
       </c>
-      <c r="C241" t="inlineStr">
+      <c r="C241" s="14" t="inlineStr">
         <is>
           <t>As a developer, I follow test-friendly patterns</t>
         </is>
       </c>
-      <c r="D241" t="inlineStr">
+      <c r="D241" s="14" t="inlineStr">
         <is>
           <t>Add data-testid attributes to critical elements</t>
         </is>
       </c>
-      <c r="E241" t="n">
+      <c r="E241" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F241" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G241" t="inlineStr">
+      <c r="F241" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G241" s="14" t="inlineStr">
         <is>
           <t>Various UI components</t>
         </is>
       </c>
-      <c r="H241" t="inlineStr">
+      <c r="H241" s="14" t="inlineStr">
         <is>
           <t>Custom test IDs for complex scenarios</t>
         </is>
       </c>
     </row>
     <row r="242">
-      <c r="A242" t="inlineStr">
+      <c r="A242" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B242" t="inlineStr">
+      <c r="B242" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Patterns</t>
         </is>
       </c>
-      <c r="C242" t="inlineStr">
+      <c r="C242" s="14" t="inlineStr">
         <is>
           <t>As a developer, I write Playwright tests</t>
         </is>
       </c>
-      <c r="D242" t="inlineStr">
+      <c r="D242" s="14" t="inlineStr">
         <is>
           <t>Page filtering tests (company, status, assignee)</t>
         </is>
       </c>
-      <c r="E242" t="n">
+      <c r="E242" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F242" t="inlineStr">
+      <c r="F242" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G242" t="inlineStr">
+      <c r="G242" s="14" t="inlineStr">
         <is>
           <t>CBaseUITest.applySearchFilter</t>
         </is>
       </c>
-      <c r="H242" t="inlineStr">
+      <c r="H242" s="14" t="inlineStr">
         <is>
           <t>Test grid filtering capabilities</t>
         </is>
       </c>
     </row>
     <row r="243">
-      <c r="A243" t="inlineStr">
+      <c r="A243" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B243" t="inlineStr">
+      <c r="B243" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Patterns</t>
         </is>
       </c>
-      <c r="C243" t="inlineStr">
+      <c r="C243" s="14" t="inlineStr">
         <is>
           <t>As a developer, I write Playwright tests</t>
         </is>
       </c>
-      <c r="D243" t="inlineStr">
+      <c r="D243" s="14" t="inlineStr">
         <is>
           <t>CRUD test pattern (direct page navigation)</t>
         </is>
       </c>
-      <c r="E243" t="n">
+      <c r="E243" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F243" t="inlineStr">
+      <c r="F243" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G243" t="inlineStr">
+      <c r="G243" s="14" t="inlineStr">
         <is>
           <t>CRecentFeaturesCrudTest</t>
         </is>
       </c>
-      <c r="H243" t="inlineStr">
+      <c r="H243" s="14" t="inlineStr">
         <is>
           <t>Create, Read, Update, Delete workflows</t>
         </is>
       </c>
     </row>
     <row r="244">
-      <c r="A244" t="inlineStr">
+      <c r="A244" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B244" t="inlineStr">
+      <c r="B244" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Patterns</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
+      <c r="C244" s="14" t="inlineStr">
         <is>
           <t>As a developer, I write Playwright tests</t>
         </is>
       </c>
-      <c r="D244" t="inlineStr">
+      <c r="D244" s="14" t="inlineStr">
         <is>
           <t>Menu navigation test pattern</t>
         </is>
       </c>
-      <c r="E244" t="n">
+      <c r="E244" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F244" t="inlineStr">
+      <c r="F244" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G244" t="inlineStr">
+      <c r="G244" s="14" t="inlineStr">
         <is>
           <t>CMenuNavigationTest</t>
         </is>
       </c>
-      <c r="H244" t="inlineStr">
+      <c r="H244" s="14" t="inlineStr">
         <is>
           <t>Hierarchical menu exploration</t>
         </is>
       </c>
     </row>
     <row r="245">
-      <c r="A245" t="inlineStr">
+      <c r="A245" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B245" t="inlineStr">
+      <c r="B245" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Patterns</t>
         </is>
       </c>
-      <c r="C245" t="inlineStr">
+      <c r="C245" s="14" t="inlineStr">
         <is>
           <t>As a developer, I write Playwright tests</t>
         </is>
       </c>
-      <c r="D245" t="inlineStr">
+      <c r="D245" s="14" t="inlineStr">
         <is>
           <t>Workflow status validation tests</t>
         </is>
       </c>
-      <c r="E245" t="n">
+      <c r="E245" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F245" t="inlineStr">
+      <c r="F245" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G245" t="inlineStr">
+      <c r="G245" s="14" t="inlineStr">
         <is>
           <t>CWorkflowStatusAndValidationTest</t>
         </is>
       </c>
-      <c r="H245" t="inlineStr">
+      <c r="H245" s="14" t="inlineStr">
         <is>
           <t>Status transitions, validation</t>
         </is>
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr">
+      <c r="A246" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B246" t="inlineStr">
+      <c r="B246" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Patterns</t>
         </is>
       </c>
-      <c r="C246" t="inlineStr">
+      <c r="C246" s="14" t="inlineStr">
         <is>
           <t>As a developer, I write Playwright tests</t>
         </is>
       </c>
-      <c r="D246" t="inlineStr">
+      <c r="D246" s="14" t="inlineStr">
         <is>
           <t>Create comprehensive test suite template</t>
         </is>
       </c>
-      <c r="E246" t="n">
+      <c r="E246" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F246" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G246" t="inlineStr">
+      <c r="F246" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G246" s="14" t="inlineStr">
         <is>
           <t>docs/testing/COMPREHENSIVE_TEST_TEMPLATE.md</t>
         </is>
       </c>
-      <c r="H246" t="inlineStr">
+      <c r="H246" s="14" t="inlineStr">
         <is>
           <t>Reusable test patterns</t>
         </is>
       </c>
     </row>
     <row r="247">
-      <c r="A247" t="inlineStr">
+      <c r="A247" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B247" t="inlineStr">
+      <c r="B247" s="14" t="inlineStr">
         <is>
           <t>Playwright Test Patterns</t>
         </is>
       </c>
-      <c r="C247" t="inlineStr">
+      <c r="C247" s="14" t="inlineStr">
         <is>
           <t>As a developer, I write Playwright tests</t>
         </is>
       </c>
-      <c r="D247" t="inlineStr">
+      <c r="D247" s="14" t="inlineStr">
         <is>
           <t>Document fail-fast exception detection</t>
         </is>
       </c>
-      <c r="E247" t="n">
+      <c r="E247" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F247" t="inlineStr">
+      <c r="F247" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G247" t="inlineStr">
+      <c r="G247" s="14" t="inlineStr">
         <is>
           <t>CBaseUITest.performFailFastCheck</t>
         </is>
       </c>
-      <c r="H247" t="inlineStr">
+      <c r="H247" s="14" t="inlineStr">
         <is>
           <t>Auto-detect exceptions in tests</t>
         </is>
       </c>
     </row>
     <row r="248">
-      <c r="A248" t="inlineStr">
+      <c r="A248" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B248" t="inlineStr">
+      <c r="B248" s="14" t="inlineStr">
         <is>
           <t>Test Coverage</t>
         </is>
       </c>
-      <c r="C248" t="inlineStr">
+      <c r="C248" s="14" t="inlineStr">
         <is>
           <t>As a manager, I want test metrics</t>
         </is>
       </c>
-      <c r="D248" t="inlineStr">
+      <c r="D248" s="14" t="inlineStr">
         <is>
           <t>Calculate test coverage by module</t>
         </is>
       </c>
-      <c r="E248" t="n">
+      <c r="E248" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F248" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G248" t="inlineStr">
+      <c r="F248" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G248" s="14" t="inlineStr">
         <is>
           <t>app.testcases.service.CTestCoverageService</t>
         </is>
       </c>
-      <c r="H248" t="inlineStr">
+      <c r="H248" s="14" t="inlineStr">
         <is>
           <t>Coverage % per project/feature</t>
         </is>
       </c>
     </row>
     <row r="249">
-      <c r="A249" t="inlineStr">
+      <c r="A249" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B249" t="inlineStr">
+      <c r="B249" s="14" t="inlineStr">
         <is>
           <t>Test Coverage</t>
         </is>
       </c>
-      <c r="C249" t="inlineStr">
+      <c r="C249" s="14" t="inlineStr">
         <is>
           <t>As a manager, I want test metrics</t>
         </is>
       </c>
-      <c r="D249" t="inlineStr">
+      <c r="D249" s="14" t="inlineStr">
         <is>
           <t>Track test execution trends</t>
         </is>
       </c>
-      <c r="E249" t="n">
+      <c r="E249" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F249" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G249" t="inlineStr">
+      <c r="F249" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G249" s="14" t="inlineStr">
         <is>
           <t>app.testcases.service.CTestMetricsService</t>
         </is>
       </c>
-      <c r="H249" t="inlineStr">
+      <c r="H249" s="14" t="inlineStr">
         <is>
           <t>Pass/fail trends over time</t>
         </is>
       </c>
     </row>
     <row r="250">
-      <c r="A250" t="inlineStr">
+      <c r="A250" s="14" t="inlineStr">
         <is>
           <t>QA &amp; Testing</t>
         </is>
       </c>
-      <c r="B250" t="inlineStr">
+      <c r="B250" s="14" t="inlineStr">
         <is>
           <t>Test Coverage</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
+      <c r="C250" s="14" t="inlineStr">
         <is>
           <t>As a manager, I want test metrics</t>
         </is>
       </c>
-      <c r="D250" t="inlineStr">
+      <c r="D250" s="14" t="inlineStr">
         <is>
           <t>Generate test execution reports</t>
         </is>
       </c>
-      <c r="E250" t="n">
+      <c r="E250" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F250" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G250" t="inlineStr">
+      <c r="F250" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G250" s="14" t="inlineStr">
         <is>
           <t>app.testcases.report.CTestExecutionReport</t>
         </is>
       </c>
-      <c r="H250" t="inlineStr">
+      <c r="H250" s="14" t="inlineStr">
         <is>
           <t>Excel/PDF export with metrics</t>
         </is>

</xml_diff>

<commit_message>
Organize test menu items under Tests parent and align with ISO/ISTQB standards terminology
Co-authored-by: yalovali <234063+yalovali@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/__PROJECT_BACKLOG.xlsx
+++ b/docs/__PROJECT_BACKLOG.xlsx
@@ -3867,250 +3867,250 @@
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1" s="15">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="14" t="inlineStr">
         <is>
           <t>Test Case Management</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="14" t="inlineStr">
         <is>
           <t>Create, read, update, delete test cases with full workflow support, test steps, and metadata</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E33" s="14" t="inlineStr">
         <is>
           <t>Users can create test cases with steps, assign types, set priority/severity, link to scenarios, view history</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" s="14" t="inlineStr">
         <is>
           <t>Views for CTestCase and CTestStep, grid with filtering, dialog forms, test step inline editor</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G33" s="14" t="inlineStr">
         <is>
           <t>CTestCase, CTestStep, CTestCaseView, CTestCaseService</t>
         </is>
       </c>
-      <c r="H33" t="n">
+      <c r="H33" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="I33" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="J33" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1" s="15">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="14" t="inlineStr">
         <is>
           <t>Test Scenario Management</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="14" t="inlineStr">
         <is>
           <t>Organize test cases into scenarios representing business workflows or features</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E34" s="14" t="inlineStr">
         <is>
           <t>Users can create scenarios, add test cases to scenarios, view scenario coverage, manage scenario lifecycle</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" s="14" t="inlineStr">
         <is>
           <t>CTestScenarioView with grid and dialog, link to test cases, scenario execution planning</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G34" s="14" t="inlineStr">
         <is>
           <t>CTestScenario, CTestScenarioView, CTestScenarioService</t>
         </is>
       </c>
-      <c r="H34" t="n">
+      <c r="H34" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="J34" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1" s="15">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="14" t="inlineStr">
         <is>
           <t>Test Execution &amp; Results</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="14" t="inlineStr">
         <is>
           <t>Execute test runs, record step-by-step results, track pass/fail metrics</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E35" s="14" t="inlineStr">
         <is>
           <t>Users can create test runs from scenarios, execute tests step-by-step, record actual results, attach evidence, view statistics</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" s="14" t="inlineStr">
         <is>
           <t>CTestRunView with execution workflow, result recording dialogs, progress tracking, metrics dashboard</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G35" s="14" t="inlineStr">
         <is>
           <t>CTestRun, CTestCaseResult, CTestStepResult, CTestRunView, CTestRunService</t>
         </is>
       </c>
-      <c r="H35" t="n">
+      <c r="H35" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="I35" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="J35" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="36" ht="13.5" customHeight="1" s="15">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="14" t="inlineStr">
         <is>
           <t>F13.4</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="14" t="inlineStr">
         <is>
           <t>Test Type Configuration</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="14" t="inlineStr">
         <is>
           <t>Configure test case types with workflows and statuses</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E36" s="14" t="inlineStr">
         <is>
           <t>Admins can create test case types, assign workflows, configure colors/icons, manage type lifecycle</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" s="14" t="inlineStr">
         <is>
           <t>CTestCaseTypeView (admin), type initializer service, workflow integration</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="G36" s="14" t="inlineStr">
         <is>
           <t>CTestCaseType, CTestCaseTypeView, CTestCaseTypeInitializerService</t>
         </is>
       </c>
-      <c r="H36" t="n">
+      <c r="H36" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="I36" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="J36" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="37" ht="13.5" customHeight="1" s="15">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="14" t="inlineStr">
         <is>
           <t>Test Reporting &amp; Analytics</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="14" t="inlineStr">
         <is>
           <t>Dashboard and reports for test metrics, coverage, trends</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E37" s="14" t="inlineStr">
         <is>
           <t>Users can view test metrics dashboard, analyze pass/fail trends, review test coverage by feature, export reports</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" s="14" t="inlineStr">
         <is>
           <t>Dashboard component, metrics calculation, chart widgets, report generation</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="G37" s="14" t="inlineStr">
         <is>
           <t>CComponentTestMetrics, CTestReportService, dashboard integration</t>
         </is>
       </c>
-      <c r="H37" t="n">
+      <c r="H37" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="I37" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="J37" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
@@ -5992,680 +5992,680 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to create test cases with detailed steps so that I can document test procedures</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="14" t="inlineStr">
         <is>
           <t>Can create test case with name, description, preconditions; Can add ordered test steps with action and expected result; Can save and view created test case</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E49" s="14" t="inlineStr">
         <is>
           <t>Use CEntityFormBuilder for test case form, embed test step grid with inline editing, validate required fields</t>
         </is>
       </c>
-      <c r="F49" t="n">
+      <c r="F49" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="H49" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="14" t="inlineStr">
         <is>
           <t>US13.1.2</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to assign priority and severity to test cases so that I can prioritize testing</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="14" t="inlineStr">
         <is>
           <t>Can select priority (LOW/MEDIUM/HIGH/CRITICAL); Can select severity (TRIVIAL/MINOR/NORMAL/MAJOR/BLOCKER); Values are saved and displayed in grid</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E50" s="14" t="inlineStr">
         <is>
           <t>Use enum fields with dropdown, display with colored badges in grid</t>
         </is>
       </c>
-      <c r="F50" t="n">
+      <c r="F50" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G50" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="H50" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="14" t="inlineStr">
         <is>
           <t>US13.1.3</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to mark test cases as automated and link to test code so that I can integrate manual and automated testing</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="14" t="inlineStr">
         <is>
           <t>Can toggle automated flag; Can enter automated test path; Automated tests are visually distinguished in grid</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E51" s="14" t="inlineStr">
         <is>
           <t>Checkbox for automated flag, text field for path, grid column renderer with icon</t>
         </is>
       </c>
-      <c r="F51" t="n">
+      <c r="F51" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="G51" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="H51" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="14" t="inlineStr">
         <is>
           <t>US13.1.4</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B52" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C52" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to view and filter test cases so that I can find relevant tests</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="D52" s="14" t="inlineStr">
         <is>
           <t>Can view all test cases in grid; Can filter by type, priority, severity, automated; Can search by name/description; Can sort by columns</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="E52" s="14" t="inlineStr">
         <is>
           <t>Use CGrid with standard filter toolbar, implement filter providers for enums</t>
         </is>
       </c>
-      <c r="F52" t="n">
+      <c r="F52" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="H52" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="14" t="inlineStr">
         <is>
           <t>US13.2.1</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B53" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C53" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to create test scenarios to group related test cases</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="D53" s="14" t="inlineStr">
         <is>
           <t>Can create scenario with name, description, objective; Can save and view scenarios in grid</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E53" s="14" t="inlineStr">
         <is>
           <t>Use standard view pattern with CGrid and dialog form</t>
         </is>
       </c>
-      <c r="F53" t="n">
+      <c r="F53" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="G53" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
+      <c r="H53" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="14" t="inlineStr">
         <is>
           <t>US13.2.2</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C54" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to add test cases to scenarios so that I can organize tests by feature</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="D54" s="14" t="inlineStr">
         <is>
           <t>Can link test case to scenario via dropdown/selector; Can view test cases grouped by scenario; Can remove test case from scenario</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E54" s="14" t="inlineStr">
         <is>
           <t>Implement entity selector in test case form, add scenario filter to test case grid</t>
         </is>
       </c>
-      <c r="F54" t="n">
+      <c r="F54" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="G54" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
+      <c r="H54" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="14" t="inlineStr">
         <is>
           <t>US13.2.3</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C55" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to view scenario completion status so that I can track testing progress</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="D55" s="14" t="inlineStr">
         <is>
           <t>Can see count of total/passed/failed test cases in scenario; Can view pass rate percentage; Status updates automatically</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E55" s="14" t="inlineStr">
         <is>
           <t>Add calculated fields to scenario entity, display in grid and detail view</t>
         </is>
       </c>
-      <c r="F55" t="n">
+      <c r="F55" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G55" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="H55" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="14" t="inlineStr">
         <is>
           <t>US13.3.1</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B56" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C56" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to create a test run from a scenario so that I can execute a group of tests</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D56" s="14" t="inlineStr">
         <is>
           <t>Can select scenario and create test run; Test run is initialized with all test cases from scenario; Can enter environment and build number</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E56" s="14" t="inlineStr">
         <is>
           <t>Create test run dialog with scenario selector, auto-populate test cases, initialize result entities</t>
         </is>
       </c>
-      <c r="F56" t="n">
+      <c r="F56" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="G56" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
+      <c r="H56" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="14" t="inlineStr">
         <is>
           <t>US13.3.2</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B57" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C57" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to execute test cases step-by-step and record results</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D57" s="14" t="inlineStr">
         <is>
           <t>Can view test case steps in execution view; Can mark each step as PASSED/FAILED/BLOCKED/SKIPPED; Can enter actual results; Can proceed to next test case</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E57" s="14" t="inlineStr">
         <is>
           <t>Create test execution component with step navigator, result recorder, progress tracker</t>
         </is>
       </c>
-      <c r="F57" t="n">
+      <c r="F57" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="G57" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
+      <c r="H57" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="14" t="inlineStr">
         <is>
           <t>US13.3.3</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B58" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C58" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to attach screenshots and logs to test results</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="D58" s="14" t="inlineStr">
         <is>
           <t>Can upload attachments during execution; Can attach files to test run or specific test case result; Attachments are linked and accessible</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E58" s="14" t="inlineStr">
         <is>
           <t>Reuse existing attachment component, link to test run and test case result entities</t>
         </is>
       </c>
-      <c r="F58" t="n">
+      <c r="F58" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G58" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
+      <c r="H58" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="14" t="inlineStr">
         <is>
           <t>US13.3.4</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B59" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="C59" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to view test run statistics so that I can assess quality</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="D59" s="14" t="inlineStr">
         <is>
           <t>Can view total/passed/failed counts for test cases and steps; Can see pass rate percentage; Can view execution duration; Statistics update in real-time</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="E59" s="14" t="inlineStr">
         <is>
           <t>Calculate and display metrics in test run view, add summary panel</t>
         </is>
       </c>
-      <c r="F59" t="n">
+      <c r="F59" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="G59" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
+      <c r="H59" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="14" t="inlineStr">
         <is>
           <t>US13.3.5</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B60" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C60" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to complete a test run and view results history</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="D60" s="14" t="inlineStr">
         <is>
           <t>Can mark test run as complete; Can view list of all test runs; Can reopen completed test runs for review; Can compare results across runs</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E60" s="14" t="inlineStr">
         <is>
           <t>Add complete button, implement test run history grid, enable result comparison view</t>
         </is>
       </c>
-      <c r="F60" t="n">
+      <c r="F60" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="G60" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
+      <c r="H60" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="14" t="inlineStr">
         <is>
           <t>US13.4.1</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B61" s="14" t="inlineStr">
         <is>
           <t>F13.4</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C61" s="14" t="inlineStr">
         <is>
           <t>As an admin, I want to configure test case types so that I can categorize tests</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="D61" s="14" t="inlineStr">
         <is>
           <t>Can create test case type with name, color, icon; Can assign workflow to type; Types appear in test case type dropdown</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="E61" s="14" t="inlineStr">
         <is>
           <t>Create admin view for test case types, reuse type entity patterns</t>
         </is>
       </c>
-      <c r="F61" t="n">
+      <c r="F61" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="G61" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
+      <c r="H61" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="14" t="inlineStr">
         <is>
           <t>US13.4.2</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B62" s="14" t="inlineStr">
         <is>
           <t>F13.4</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C62" s="14" t="inlineStr">
         <is>
           <t>As an admin, I want to define workflows for test case types</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="D62" s="14" t="inlineStr">
         <is>
           <t>Can select workflow for each type; Test cases follow assigned workflow statuses; Workflow rules apply to test cases of that type</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E62" s="14" t="inlineStr">
         <is>
           <t>Workflow assignment in type entity, enforce workflow in test case service</t>
         </is>
       </c>
-      <c r="F62" t="n">
+      <c r="F62" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="G62" s="14" t="inlineStr">
         <is>
           <t>LOW</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
+      <c r="H62" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
+      <c r="A63" s="14" t="inlineStr">
         <is>
           <t>US13.5.1</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B63" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C63" s="14" t="inlineStr">
         <is>
           <t>As a project manager, I want to view a test metrics dashboard</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="D63" s="14" t="inlineStr">
         <is>
           <t>Can view overall test coverage metrics; Can see pass/fail trends over time; Can drill down into failed tests</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E63" s="14" t="inlineStr">
         <is>
           <t>Create dashboard component with charts and metrics, integrate with project dashboard</t>
         </is>
       </c>
-      <c r="F63" t="n">
+      <c r="F63" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="G63" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
+      <c r="H63" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="14" t="inlineStr">
         <is>
           <t>US13.5.2</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B64" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="C64" s="14" t="inlineStr">
         <is>
           <t>As a project manager, I want to export test reports</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="D64" s="14" t="inlineStr">
         <is>
           <t>Can generate test summary report; Can export to PDF or Excel; Report includes all test run details and statistics</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="E64" s="14" t="inlineStr">
         <is>
           <t>Implement report generation service, add export buttons to test run view</t>
         </is>
       </c>
-      <c r="F64" t="n">
+      <c r="F64" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="G64" s="14" t="inlineStr">
         <is>
           <t>LOW</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr">
+      <c r="H64" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="14" t="inlineStr">
         <is>
           <t>US13.5.3</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B65" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C65" s="14" t="inlineStr">
         <is>
           <t>As a QA engineer, I want to see test coverage by feature</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="D65" s="14" t="inlineStr">
         <is>
           <t>Can view which features have test coverage; Can identify gaps in test coverage; Coverage percentage is calculated automatically</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="E65" s="14" t="inlineStr">
         <is>
           <t>Link test scenarios to features, calculate coverage metrics, display coverage matrix</t>
         </is>
       </c>
-      <c r="F65" t="n">
+      <c r="F65" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="G65" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
+      <c r="H65" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
@@ -6685,7 +6685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I250"/>
+  <dimension ref="A1:I271"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
@@ -16746,6 +16746,846 @@
       <c r="H250" s="14" t="inlineStr">
         <is>
           <t>Excel/PDF export with metrics</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Add MenuTitle_TESTS and Menu_Order_TESTS constants to CInitializerServiceBase</t>
+        </is>
+      </c>
+      <c r="E251" t="n">
+        <v>1</v>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>CInitializerServiceBase</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>Added constants for Tests menu organization</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Update CTestCaseInitializerService to use MenuTitle_TESTS parent menu</t>
+        </is>
+      </c>
+      <c r="E252" t="n">
+        <v>1</v>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>CTestCaseInitializerService</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>Changed from Project.Test Cases to Tests.Test Cases</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>US13.2.1</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Update CTestScenarioInitializerService to use MenuTitle_TESTS parent menu</t>
+        </is>
+      </c>
+      <c r="E253" t="n">
+        <v>1</v>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>CTestScenarioInitializerService</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>Changed from Project.Test Scenarios to Tests.Test Scenarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>US13.3.1</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Update CTestRunInitializerService to use MenuTitle_TESTS parent menu</t>
+        </is>
+      </c>
+      <c r="E254" t="n">
+        <v>1</v>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>CTestRunInitializerService</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>Changed from Project.Test Runs to Tests.Test Runs</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>US13.1.4</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Verify test pages appear in Tests menu after project creation</t>
+        </is>
+      </c>
+      <c r="E255" t="n">
+        <v>2</v>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>Manual testing</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>Create new project and verify Tests menu structure</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Test CRUD operations on CTestCase entities</t>
+        </is>
+      </c>
+      <c r="E256" t="n">
+        <v>3</v>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>UI testing</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>Create, read, update, delete test cases; verify test steps inline editing</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>US13.2.2</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Test linking test cases to scenarios</t>
+        </is>
+      </c>
+      <c r="E257" t="n">
+        <v>2</v>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>UI testing</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>Create scenario, link test cases, verify relationship</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>US13.3.2</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Test test run execution workflow</t>
+        </is>
+      </c>
+      <c r="E258" t="n">
+        <v>3</v>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>UI testing</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>Create test run, execute test cases step-by-step, record results</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>US13.3.3</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Test attachment upload during test execution</t>
+        </is>
+      </c>
+      <c r="E259" t="n">
+        <v>2</v>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>UI testing</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>Upload screenshots and logs to test runs and results</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>US13.3.2</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Create test execution component for step-by-step testing</t>
+        </is>
+      </c>
+      <c r="E260" t="n">
+        <v>8</v>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>CComponentTestExecution</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>Component for executing tests with step navigation and result recording</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>US13.5.1</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Create test metrics dashboard component</t>
+        </is>
+      </c>
+      <c r="E261" t="n">
+        <v>5</v>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>CComponentTestMetrics</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>Dashboard widget showing test coverage and pass/fail metrics</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>US13.5.2</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Implement test report generation service</t>
+        </is>
+      </c>
+      <c r="E262" t="n">
+        <v>5</v>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>CTestReportService</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>Generate PDF/Excel reports from test runs</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Create testing methodology architecture documentation</t>
+        </is>
+      </c>
+      <c r="E263" t="n">
+        <v>1</v>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>docs/architecture/TESTING_METHODOLOGY.md</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>Comprehensive testing methodology guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Create testing standards compliance documentation</t>
+        </is>
+      </c>
+      <c r="E264" t="n">
+        <v>1</v>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>docs/testing/TESTING_STANDARDS_COMPLIANCE.md</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>ISO/ISTQB/ProjeQtOr compliance documentation</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Update project backlog with testing tasks</t>
+        </is>
+      </c>
+      <c r="E265" t="n">
+        <v>1</v>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>docs/__PROJECT_BACKLOG.xlsx</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>Added features, stories, and tasks for testing module</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>US13.1.4</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Create Playwright tests for Test Cases CRUD</t>
+        </is>
+      </c>
+      <c r="E266" t="n">
+        <v>3</v>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>CTestCaseCRUDTest</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>Automated UI tests for test case management</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>US13.2.1</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Create Playwright tests for Test Scenarios CRUD</t>
+        </is>
+      </c>
+      <c r="E267" t="n">
+        <v>3</v>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>CTestScenarioCRUDTest</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>Automated UI tests for test scenario management</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>US13.3.1</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Create Playwright tests for Test Run creation and execution</t>
+        </is>
+      </c>
+      <c r="E268" t="n">
+        <v>5</v>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>CTestRunExecutionTest</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>Automated UI tests for test execution workflow</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>US13.1.3</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Add visual indicators for automated vs manual tests in grid</t>
+        </is>
+      </c>
+      <c r="E269" t="n">
+        <v>1</v>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>CTestCaseInitializerService</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>Add icon/badge renderer for automated flag</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>US13.3.4</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Add real-time statistics calculation in test runs</t>
+        </is>
+      </c>
+      <c r="E270" t="n">
+        <v>2</v>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>CTestRunService</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>Calculate pass/fail rates as tests are executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>US13.5.3</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Implement test coverage matrix by feature</t>
+        </is>
+      </c>
+      <c r="E271" t="n">
+        <v>5</v>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>CTestCoverageService</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>Link scenarios to features and calculate coverage</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete pattern compliance audit and update project backlog with implementation status
Co-authored-by: yalovali <234063+yalovali@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/__PROJECT_BACKLOG.xlsx
+++ b/docs/__PROJECT_BACKLOG.xlsx
@@ -6685,7 +6685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I271"/>
+  <dimension ref="A1:I289"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
@@ -15775,7 +15775,7 @@
       </c>
       <c r="F226" s="14" t="inlineStr">
         <is>
-          <t>TODO</t>
+          <t>DONE</t>
         </is>
       </c>
       <c r="G226" s="14" t="inlineStr">
@@ -15785,7 +15785,7 @@
       </c>
       <c r="H226" s="14" t="inlineStr">
         <is>
-          <t>CRUD, reordering steps</t>
+          <t>Completed - 2026-01-16</t>
         </is>
       </c>
     </row>
@@ -16750,842 +16750,1562 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" t="inlineStr">
+      <c r="A251" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B251" t="inlineStr">
+      <c r="B251" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C251" t="inlineStr">
+      <c r="C251" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D251" t="inlineStr">
+      <c r="D251" s="14" t="inlineStr">
         <is>
           <t>Add MenuTitle_TESTS and Menu_Order_TESTS constants to CInitializerServiceBase</t>
         </is>
       </c>
-      <c r="E251" t="n">
+      <c r="E251" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F251" t="inlineStr">
+      <c r="F251" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G251" t="inlineStr">
+      <c r="G251" s="14" t="inlineStr">
         <is>
           <t>CInitializerServiceBase</t>
         </is>
       </c>
-      <c r="H251" t="inlineStr">
+      <c r="H251" s="14" t="inlineStr">
         <is>
           <t>Added constants for Tests menu organization</t>
         </is>
       </c>
     </row>
     <row r="252">
-      <c r="A252" t="inlineStr">
+      <c r="A252" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B252" t="inlineStr">
+      <c r="B252" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C252" t="inlineStr">
+      <c r="C252" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D252" t="inlineStr">
+      <c r="D252" s="14" t="inlineStr">
         <is>
           <t>Update CTestCaseInitializerService to use MenuTitle_TESTS parent menu</t>
         </is>
       </c>
-      <c r="E252" t="n">
+      <c r="E252" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F252" t="inlineStr">
+      <c r="F252" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G252" t="inlineStr">
+      <c r="G252" s="14" t="inlineStr">
         <is>
           <t>CTestCaseInitializerService</t>
         </is>
       </c>
-      <c r="H252" t="inlineStr">
+      <c r="H252" s="14" t="inlineStr">
         <is>
           <t>Changed from Project.Test Cases to Tests.Test Cases</t>
         </is>
       </c>
     </row>
     <row r="253">
-      <c r="A253" t="inlineStr">
+      <c r="A253" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B253" t="inlineStr">
+      <c r="B253" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="C253" t="inlineStr">
+      <c r="C253" s="14" t="inlineStr">
         <is>
           <t>US13.2.1</t>
         </is>
       </c>
-      <c r="D253" t="inlineStr">
+      <c r="D253" s="14" t="inlineStr">
         <is>
           <t>Update CTestScenarioInitializerService to use MenuTitle_TESTS parent menu</t>
         </is>
       </c>
-      <c r="E253" t="n">
+      <c r="E253" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F253" t="inlineStr">
+      <c r="F253" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G253" t="inlineStr">
+      <c r="G253" s="14" t="inlineStr">
         <is>
           <t>CTestScenarioInitializerService</t>
         </is>
       </c>
-      <c r="H253" t="inlineStr">
+      <c r="H253" s="14" t="inlineStr">
         <is>
           <t>Changed from Project.Test Scenarios to Tests.Test Scenarios</t>
         </is>
       </c>
     </row>
     <row r="254">
-      <c r="A254" t="inlineStr">
+      <c r="A254" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B254" t="inlineStr">
+      <c r="B254" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C254" t="inlineStr">
+      <c r="C254" s="14" t="inlineStr">
         <is>
           <t>US13.3.1</t>
         </is>
       </c>
-      <c r="D254" t="inlineStr">
+      <c r="D254" s="14" t="inlineStr">
         <is>
           <t>Update CTestRunInitializerService to use MenuTitle_TESTS parent menu</t>
         </is>
       </c>
-      <c r="E254" t="n">
+      <c r="E254" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F254" t="inlineStr">
+      <c r="F254" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G254" t="inlineStr">
+      <c r="G254" s="14" t="inlineStr">
         <is>
           <t>CTestRunInitializerService</t>
         </is>
       </c>
-      <c r="H254" t="inlineStr">
+      <c r="H254" s="14" t="inlineStr">
         <is>
           <t>Changed from Project.Test Runs to Tests.Test Runs</t>
         </is>
       </c>
     </row>
     <row r="255">
-      <c r="A255" t="inlineStr">
+      <c r="A255" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B255" t="inlineStr">
+      <c r="B255" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C255" t="inlineStr">
+      <c r="C255" s="14" t="inlineStr">
         <is>
           <t>US13.1.4</t>
         </is>
       </c>
-      <c r="D255" t="inlineStr">
+      <c r="D255" s="14" t="inlineStr">
         <is>
           <t>Verify test pages appear in Tests menu after project creation</t>
         </is>
       </c>
-      <c r="E255" t="n">
+      <c r="E255" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F255" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G255" t="inlineStr">
+      <c r="F255" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G255" s="14" t="inlineStr">
         <is>
           <t>Manual testing</t>
         </is>
       </c>
-      <c r="H255" t="inlineStr">
+      <c r="H255" s="14" t="inlineStr">
         <is>
           <t>Create new project and verify Tests menu structure</t>
         </is>
       </c>
     </row>
     <row r="256">
-      <c r="A256" t="inlineStr">
+      <c r="A256" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B256" t="inlineStr">
+      <c r="B256" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C256" t="inlineStr">
+      <c r="C256" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D256" t="inlineStr">
+      <c r="D256" s="14" t="inlineStr">
         <is>
           <t>Test CRUD operations on CTestCase entities</t>
         </is>
       </c>
-      <c r="E256" t="n">
+      <c r="E256" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F256" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G256" t="inlineStr">
+      <c r="F256" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G256" s="14" t="inlineStr">
         <is>
           <t>UI testing</t>
         </is>
       </c>
-      <c r="H256" t="inlineStr">
+      <c r="H256" s="14" t="inlineStr">
         <is>
           <t>Create, read, update, delete test cases; verify test steps inline editing</t>
         </is>
       </c>
     </row>
     <row r="257">
-      <c r="A257" t="inlineStr">
+      <c r="A257" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B257" t="inlineStr">
+      <c r="B257" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="C257" t="inlineStr">
+      <c r="C257" s="14" t="inlineStr">
         <is>
           <t>US13.2.2</t>
         </is>
       </c>
-      <c r="D257" t="inlineStr">
+      <c r="D257" s="14" t="inlineStr">
         <is>
           <t>Test linking test cases to scenarios</t>
         </is>
       </c>
-      <c r="E257" t="n">
+      <c r="E257" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F257" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G257" t="inlineStr">
+      <c r="F257" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G257" s="14" t="inlineStr">
         <is>
           <t>UI testing</t>
         </is>
       </c>
-      <c r="H257" t="inlineStr">
+      <c r="H257" s="14" t="inlineStr">
         <is>
           <t>Create scenario, link test cases, verify relationship</t>
         </is>
       </c>
     </row>
     <row r="258">
-      <c r="A258" t="inlineStr">
+      <c r="A258" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B258" t="inlineStr">
+      <c r="B258" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C258" t="inlineStr">
+      <c r="C258" s="14" t="inlineStr">
         <is>
           <t>US13.3.2</t>
         </is>
       </c>
-      <c r="D258" t="inlineStr">
+      <c r="D258" s="14" t="inlineStr">
         <is>
           <t>Test test run execution workflow</t>
         </is>
       </c>
-      <c r="E258" t="n">
+      <c r="E258" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F258" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G258" t="inlineStr">
+      <c r="F258" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G258" s="14" t="inlineStr">
         <is>
           <t>UI testing</t>
         </is>
       </c>
-      <c r="H258" t="inlineStr">
+      <c r="H258" s="14" t="inlineStr">
         <is>
           <t>Create test run, execute test cases step-by-step, record results</t>
         </is>
       </c>
     </row>
     <row r="259">
-      <c r="A259" t="inlineStr">
+      <c r="A259" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B259" t="inlineStr">
+      <c r="B259" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C259" t="inlineStr">
+      <c r="C259" s="14" t="inlineStr">
         <is>
           <t>US13.3.3</t>
         </is>
       </c>
-      <c r="D259" t="inlineStr">
+      <c r="D259" s="14" t="inlineStr">
         <is>
           <t>Test attachment upload during test execution</t>
         </is>
       </c>
-      <c r="E259" t="n">
+      <c r="E259" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F259" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G259" t="inlineStr">
+      <c r="F259" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G259" s="14" t="inlineStr">
         <is>
           <t>UI testing</t>
         </is>
       </c>
-      <c r="H259" t="inlineStr">
+      <c r="H259" s="14" t="inlineStr">
         <is>
           <t>Upload screenshots and logs to test runs and results</t>
         </is>
       </c>
     </row>
     <row r="260">
-      <c r="A260" t="inlineStr">
+      <c r="A260" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B260" t="inlineStr">
+      <c r="B260" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C260" t="inlineStr">
+      <c r="C260" s="14" t="inlineStr">
         <is>
           <t>US13.3.2</t>
         </is>
       </c>
-      <c r="D260" t="inlineStr">
+      <c r="D260" s="14" t="inlineStr">
         <is>
           <t>Create test execution component for step-by-step testing</t>
         </is>
       </c>
-      <c r="E260" t="n">
+      <c r="E260" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F260" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G260" t="inlineStr">
+      <c r="F260" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G260" s="14" t="inlineStr">
         <is>
           <t>CComponentTestExecution</t>
         </is>
       </c>
-      <c r="H260" t="inlineStr">
+      <c r="H260" s="14" t="inlineStr">
         <is>
           <t>Component for executing tests with step navigation and result recording</t>
         </is>
       </c>
     </row>
     <row r="261">
-      <c r="A261" t="inlineStr">
+      <c r="A261" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B261" t="inlineStr">
+      <c r="B261" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C261" t="inlineStr">
+      <c r="C261" s="14" t="inlineStr">
         <is>
           <t>US13.5.1</t>
         </is>
       </c>
-      <c r="D261" t="inlineStr">
+      <c r="D261" s="14" t="inlineStr">
         <is>
           <t>Create test metrics dashboard component</t>
         </is>
       </c>
-      <c r="E261" t="n">
+      <c r="E261" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F261" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G261" t="inlineStr">
+      <c r="F261" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G261" s="14" t="inlineStr">
         <is>
           <t>CComponentTestMetrics</t>
         </is>
       </c>
-      <c r="H261" t="inlineStr">
+      <c r="H261" s="14" t="inlineStr">
         <is>
           <t>Dashboard widget showing test coverage and pass/fail metrics</t>
         </is>
       </c>
     </row>
     <row r="262">
-      <c r="A262" t="inlineStr">
+      <c r="A262" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B262" t="inlineStr">
+      <c r="B262" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C262" t="inlineStr">
+      <c r="C262" s="14" t="inlineStr">
         <is>
           <t>US13.5.2</t>
         </is>
       </c>
-      <c r="D262" t="inlineStr">
+      <c r="D262" s="14" t="inlineStr">
         <is>
           <t>Implement test report generation service</t>
         </is>
       </c>
-      <c r="E262" t="n">
+      <c r="E262" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F262" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G262" t="inlineStr">
+      <c r="F262" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G262" s="14" t="inlineStr">
         <is>
           <t>CTestReportService</t>
         </is>
       </c>
-      <c r="H262" t="inlineStr">
+      <c r="H262" s="14" t="inlineStr">
         <is>
           <t>Generate PDF/Excel reports from test runs</t>
         </is>
       </c>
     </row>
     <row r="263">
-      <c r="A263" t="inlineStr">
+      <c r="A263" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B263" t="inlineStr">
+      <c r="B263" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C263" t="inlineStr">
+      <c r="C263" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D263" t="inlineStr">
+      <c r="D263" s="14" t="inlineStr">
         <is>
           <t>Create testing methodology architecture documentation</t>
         </is>
       </c>
-      <c r="E263" t="n">
+      <c r="E263" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F263" t="inlineStr">
+      <c r="F263" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G263" t="inlineStr">
+      <c r="G263" s="14" t="inlineStr">
         <is>
           <t>docs/architecture/TESTING_METHODOLOGY.md</t>
         </is>
       </c>
-      <c r="H263" t="inlineStr">
+      <c r="H263" s="14" t="inlineStr">
         <is>
           <t>Comprehensive testing methodology guide</t>
         </is>
       </c>
     </row>
     <row r="264">
-      <c r="A264" t="inlineStr">
+      <c r="A264" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B264" t="inlineStr">
+      <c r="B264" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C264" t="inlineStr">
+      <c r="C264" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D264" t="inlineStr">
+      <c r="D264" s="14" t="inlineStr">
         <is>
           <t>Create testing standards compliance documentation</t>
         </is>
       </c>
-      <c r="E264" t="n">
+      <c r="E264" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F264" t="inlineStr">
+      <c r="F264" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G264" t="inlineStr">
+      <c r="G264" s="14" t="inlineStr">
         <is>
           <t>docs/testing/TESTING_STANDARDS_COMPLIANCE.md</t>
         </is>
       </c>
-      <c r="H264" t="inlineStr">
+      <c r="H264" s="14" t="inlineStr">
         <is>
           <t>ISO/ISTQB/ProjeQtOr compliance documentation</t>
         </is>
       </c>
     </row>
     <row r="265">
-      <c r="A265" t="inlineStr">
+      <c r="A265" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B265" t="inlineStr">
+      <c r="B265" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C265" t="inlineStr">
+      <c r="C265" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D265" t="inlineStr">
+      <c r="D265" s="14" t="inlineStr">
         <is>
           <t>Update project backlog with testing tasks</t>
         </is>
       </c>
-      <c r="E265" t="n">
+      <c r="E265" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F265" t="inlineStr">
+      <c r="F265" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G265" t="inlineStr">
+      <c r="G265" s="14" t="inlineStr">
         <is>
           <t>docs/__PROJECT_BACKLOG.xlsx</t>
         </is>
       </c>
-      <c r="H265" t="inlineStr">
+      <c r="H265" s="14" t="inlineStr">
         <is>
           <t>Added features, stories, and tasks for testing module</t>
         </is>
       </c>
     </row>
     <row r="266">
-      <c r="A266" t="inlineStr">
+      <c r="A266" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B266" t="inlineStr">
+      <c r="B266" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C266" t="inlineStr">
+      <c r="C266" s="14" t="inlineStr">
         <is>
           <t>US13.1.4</t>
         </is>
       </c>
-      <c r="D266" t="inlineStr">
+      <c r="D266" s="14" t="inlineStr">
         <is>
           <t>Create Playwright tests for Test Cases CRUD</t>
         </is>
       </c>
-      <c r="E266" t="n">
+      <c r="E266" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F266" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G266" t="inlineStr">
+      <c r="F266" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G266" s="14" t="inlineStr">
         <is>
           <t>CTestCaseCRUDTest</t>
         </is>
       </c>
-      <c r="H266" t="inlineStr">
+      <c r="H266" s="14" t="inlineStr">
         <is>
           <t>Automated UI tests for test case management</t>
         </is>
       </c>
     </row>
     <row r="267">
-      <c r="A267" t="inlineStr">
+      <c r="A267" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B267" t="inlineStr">
+      <c r="B267" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="C267" t="inlineStr">
+      <c r="C267" s="14" t="inlineStr">
         <is>
           <t>US13.2.1</t>
         </is>
       </c>
-      <c r="D267" t="inlineStr">
+      <c r="D267" s="14" t="inlineStr">
         <is>
           <t>Create Playwright tests for Test Scenarios CRUD</t>
         </is>
       </c>
-      <c r="E267" t="n">
+      <c r="E267" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F267" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G267" t="inlineStr">
+      <c r="F267" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G267" s="14" t="inlineStr">
         <is>
           <t>CTestScenarioCRUDTest</t>
         </is>
       </c>
-      <c r="H267" t="inlineStr">
+      <c r="H267" s="14" t="inlineStr">
         <is>
           <t>Automated UI tests for test scenario management</t>
         </is>
       </c>
     </row>
     <row r="268">
-      <c r="A268" t="inlineStr">
+      <c r="A268" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B268" t="inlineStr">
+      <c r="B268" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C268" t="inlineStr">
+      <c r="C268" s="14" t="inlineStr">
         <is>
           <t>US13.3.1</t>
         </is>
       </c>
-      <c r="D268" t="inlineStr">
+      <c r="D268" s="14" t="inlineStr">
         <is>
           <t>Create Playwright tests for Test Run creation and execution</t>
         </is>
       </c>
-      <c r="E268" t="n">
+      <c r="E268" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F268" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G268" t="inlineStr">
+      <c r="F268" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G268" s="14" t="inlineStr">
         <is>
           <t>CTestRunExecutionTest</t>
         </is>
       </c>
-      <c r="H268" t="inlineStr">
+      <c r="H268" s="14" t="inlineStr">
         <is>
           <t>Automated UI tests for test execution workflow</t>
         </is>
       </c>
     </row>
     <row r="269">
-      <c r="A269" t="inlineStr">
+      <c r="A269" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B269" t="inlineStr">
+      <c r="B269" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C269" t="inlineStr">
+      <c r="C269" s="14" t="inlineStr">
         <is>
           <t>US13.1.3</t>
         </is>
       </c>
-      <c r="D269" t="inlineStr">
+      <c r="D269" s="14" t="inlineStr">
         <is>
           <t>Add visual indicators for automated vs manual tests in grid</t>
         </is>
       </c>
-      <c r="E269" t="n">
+      <c r="E269" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F269" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G269" t="inlineStr">
+      <c r="F269" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G269" s="14" t="inlineStr">
         <is>
           <t>CTestCaseInitializerService</t>
         </is>
       </c>
-      <c r="H269" t="inlineStr">
+      <c r="H269" s="14" t="inlineStr">
         <is>
           <t>Add icon/badge renderer for automated flag</t>
         </is>
       </c>
     </row>
     <row r="270">
-      <c r="A270" t="inlineStr">
+      <c r="A270" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B270" t="inlineStr">
+      <c r="B270" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C270" t="inlineStr">
+      <c r="C270" s="14" t="inlineStr">
         <is>
           <t>US13.3.4</t>
         </is>
       </c>
-      <c r="D270" t="inlineStr">
+      <c r="D270" s="14" t="inlineStr">
         <is>
           <t>Add real-time statistics calculation in test runs</t>
         </is>
       </c>
-      <c r="E270" t="n">
+      <c r="E270" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F270" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G270" t="inlineStr">
+      <c r="F270" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G270" s="14" t="inlineStr">
         <is>
           <t>CTestRunService</t>
         </is>
       </c>
-      <c r="H270" t="inlineStr">
+      <c r="H270" s="14" t="inlineStr">
         <is>
           <t>Calculate pass/fail rates as tests are executed</t>
         </is>
       </c>
     </row>
     <row r="271">
-      <c r="A271" t="inlineStr">
+      <c r="A271" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B271" t="inlineStr">
+      <c r="B271" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C271" t="inlineStr">
+      <c r="C271" s="14" t="inlineStr">
         <is>
           <t>US13.5.3</t>
         </is>
       </c>
-      <c r="D271" t="inlineStr">
+      <c r="D271" s="14" t="inlineStr">
         <is>
           <t>Implement test coverage matrix by feature</t>
         </is>
       </c>
-      <c r="E271" t="n">
+      <c r="E271" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F271" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G271" t="inlineStr">
+      <c r="F271" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G271" s="14" t="inlineStr">
         <is>
           <t>CTestCoverageService</t>
         </is>
       </c>
-      <c r="H271" t="inlineStr">
+      <c r="H271" s="14" t="inlineStr">
         <is>
           <t>Link scenarios to features and calculate coverage</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>US13.3.2</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Implement CComponentTestExecution - main execution interface</t>
+        </is>
+      </c>
+      <c r="E272" t="n">
+        <v>8</v>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>CComponentTestExecution.java</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>933 lines - Auto-save, keyboard shortcuts, ISO compliance - 2026-01-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>US13.3.2</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Update CPageServiceTestRun with component factory method</t>
+        </is>
+      </c>
+      <c r="E273" t="n">
+        <v>1</v>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>CPageServiceTestRun.java</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>createTestExecutionComponent() added - 2026-01-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>US13.3.3</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Add single-page execution view to CTestRunInitializerService</t>
+        </is>
+      </c>
+      <c r="E274" t="n">
+        <v>2</v>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>IN_PROGRESS</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>CTestRunInitializerService.java</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>Add second view with setAttributeNone(true) for full-screen execution</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>US13.3.3</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Add Execute button to test run detail view</t>
+        </is>
+      </c>
+      <c r="E275" t="n">
+        <v>1</v>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>Test run detail</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>Launch button for execution interface</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>US13.3.4</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Integrate screenshot capture functionality</t>
+        </is>
+      </c>
+      <c r="E276" t="n">
+        <v>3</v>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>CComponentTestExecution</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>Browser screenshot API for evidence</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>US13.3.4</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Implement file attachment upload in execution</t>
+        </is>
+      </c>
+      <c r="E277" t="n">
+        <v>2</v>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>CComponentTestExecution</t>
+        </is>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>Drag-drop file upload integration</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>US13.1.4</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Playwright: Test Cases CRUD operations</t>
+        </is>
+      </c>
+      <c r="E278" t="n">
+        <v>3</v>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>automated_tests/</t>
+        </is>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>Create, read, update, delete test cases</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>F13.2</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>US13.2.1</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Playwright: Test Suites CRUD operations</t>
+        </is>
+      </c>
+      <c r="E279" t="n">
+        <v>3</v>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>automated_tests/</t>
+        </is>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>Create, read, update, delete test suites</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>US13.3.1</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Playwright: Test Session creation workflow</t>
+        </is>
+      </c>
+      <c r="E280" t="n">
+        <v>2</v>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>automated_tests/</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>Create session, link to suite</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>US13.3.2</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Playwright: Complete test execution workflow</t>
+        </is>
+      </c>
+      <c r="E281" t="n">
+        <v>5</v>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>automated_tests/</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>Execute test, record results, validate statistics</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>F13.3</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>US13.3.5</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Playwright: Result recording validation</t>
+        </is>
+      </c>
+      <c r="E282" t="n">
+        <v>3</v>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>automated_tests/</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>Test PASS/FAIL/SKIP/BLOCK recording</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>US13.5.1</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Create test metrics dashboard component</t>
+        </is>
+      </c>
+      <c r="E283" t="n">
+        <v>5</v>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>CComponentTestMetrics</t>
+        </is>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>Charts: pass rate, coverage, trends</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>US13.5.2</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Implement test report generation service</t>
+        </is>
+      </c>
+      <c r="E284" t="n">
+        <v>5</v>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>CTestReportService</t>
+        </is>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>Export to PDF/Excel with charts</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>F13.5</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>US13.5.3</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Implement test coverage matrix by feature</t>
+        </is>
+      </c>
+      <c r="E285" t="n">
+        <v>5</v>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>CTestCoverageService</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>Link test cases to requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Run Spotless formatter on all test files</t>
+        </is>
+      </c>
+      <c r="E286" t="n">
+        <v>1</v>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>Maven spotless:apply</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>Format Java files to coding standards</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Run CodeQL security scan</t>
+        </is>
+      </c>
+      <c r="E287" t="n">
+        <v>1</v>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>GitHub Actions</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>Security vulnerability check</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Update terminology with ISO/ISTQB UI standards</t>
+        </is>
+      </c>
+      <c r="E288" t="n">
+        <v>1</v>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>TESTING_TERMINOLOGY_MAPPING.md</t>
+        </is>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>UI component standards added - 2026-01-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>E13</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>F13.1</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>US13.1.1</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Create code pattern compliance audit</t>
+        </is>
+      </c>
+      <c r="E289" t="n">
+        <v>1</v>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>CODE_PATTERN_COMPLIANCE_AUDIT.md</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>100% pattern compliance verified - 2026-01-16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add CRM module: Customer and CustomerType entities with full service layer
Co-authored-by: yalovali <234063+yalovali@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/__PROJECT_BACKLOG.xlsx
+++ b/docs/__PROJECT_BACKLOG.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
@@ -2175,6 +2175,72 @@
         <v/>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>E32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CRM &amp; Customer Relationship Management</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Complete CRM system with customer/account management, contact tracking, lead management, opportunity/deal pipeline, sales funnel visualization, customer interactions, and customer analytics. Enables comprehensive customer lifecycle management.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Enables customer-centric operations, improves sales pipeline visibility, tracks customer interactions, forecasts revenue, manages customer lifecycle, supports sales team efficiency, provides customer insights and analytics.</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Not Implemented</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>customers, contacts, leads, opportunities, deals, salespipeline</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="K33">
+        <f>SUMIF(Features!B:B,A33,Features!I:I)</f>
+        <v/>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G15"/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -2189,7 +2255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
@@ -4116,12 +4182,300 @@
         </is>
       </c>
     </row>
-    <row r="38" ht="13.5" customHeight="1" s="15"/>
-    <row r="39" ht="13.5" customHeight="1" s="15"/>
-    <row r="40" ht="13.5" customHeight="1" s="15"/>
-    <row r="41" ht="13.5" customHeight="1" s="15"/>
-    <row r="42" ht="13.5" customHeight="1" s="15"/>
-    <row r="43" ht="13.5" customHeight="1" s="15"/>
+    <row r="38" ht="13.5" customHeight="1" s="15">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>E32F1</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>E32</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Customer &amp; Account Management</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Comprehensive customer/account entity with company details, industry classification, relationship type, customer status, revenue tracking, and customer lifecycle management.</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Centralizes customer data, tracks customer health, manages customer hierarchy, supports account-based selling.</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>customers.customer, customers.customertype</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <f>SUMIF(User_Stories!B:B,A38,User_Stories!H:H)</f>
+        <v/>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="13.5" customHeight="1" s="15">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>E32F2</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>E32</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Contact Management</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Individual contact records linked to customers with full contact details, role/title tracking, communication preferences, interaction history, and relationship strength scoring.</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Enables person-level relationship tracking, manages contact hierarchies, tracks communication preferences, improves outreach effectiveness.</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>contacts.contact, contacts.contacttype</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <f>SUMIF(User_Stories!B:B,A39,User_Stories!H:H)</f>
+        <v/>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="13.5" customHeight="1" s="15">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>E32F3</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>E32</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Lead Management &amp; Qualification</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Lead capture, scoring, qualification, and conversion tracking. Manages leads from first contact through qualification to opportunity conversion.</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Captures early-stage prospects, prioritizes leads by score, tracks lead sources, measures conversion rates, prevents lead leakage.</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>leads.lead, leads.leadsource, leads.leadstatus</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <f>SUMIF(User_Stories!B:B,A40,User_Stories!H:H)</f>
+        <v/>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="13.5" customHeight="1" s="15">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>E32F4</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>E32</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Opportunity &amp; Deal Pipeline Management</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Sales opportunity tracking with pipeline stages, probability tracking, expected close dates, deal value, competitive tracking, and win/loss analysis.</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Visualizes sales pipeline, forecasts revenue, tracks deal progress, identifies bottlenecks, improves win rates through analysis.</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>opportunities.opportunity, opportunities.opportunitystage, opportunities.winlossreason</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <f>SUMIF(User_Stories!B:B,A41,User_Stories!H:H)</f>
+        <v/>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>CRITICAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="13.5" customHeight="1" s="15">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>E32F5</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>E32</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Sales Funnel &amp; Pipeline Analytics</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Visual sales funnel showing conversion rates between stages, pipeline value analysis, forecast accuracy tracking, and sales velocity metrics.</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Identifies pipeline bottlenecks, forecasts revenue accurately, measures sales efficiency, tracks conversion rates, supports data-driven sales decisions.</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>pipeline.dashboard, pipeline.funnel</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <f>SUMIF(User_Stories!B:B,A42,User_Stories!H:H)</f>
+        <v/>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="13.5" customHeight="1" s="15">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>E32F6</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>E32</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Customer Interaction &amp; Activity Tracking</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Log and track all customer touchpoints including calls, emails, meetings, demos, and custom activities. Maintains complete interaction history per customer.</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Provides 360° customer view, improves handoffs, tracks engagement frequency, ensures follow-up, supports relationship quality scoring.</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Leverage existing CActivity and CMeeting</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <f>SUMIF(User_Stories!B:B,A43,User_Stories!H:H)</f>
+        <v/>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
     <row r="44" ht="13.5" customHeight="1" s="15"/>
     <row r="45" ht="13.5" customHeight="1" s="15"/>
     <row r="46" ht="13.5" customHeight="1" s="15"/>
@@ -4142,7 +4496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
@@ -6668,6 +7022,726 @@
       <c r="H65" s="14" t="inlineStr">
         <is>
           <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>E32F1S1</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>E32F1</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>As a sales manager, I want to create and manage customer accounts with detailed company information</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Create CCustomer entity with fields: company name, industry, size, website, revenue, customer type, status, relationship start date, description, logo. Extends CProjectItem. Implements IHasStatusAndWorkflow, IHasAttachments, IHasComments.</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>customers.customer.domain.CCustomer</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>5</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>CRITICAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>E32F1S2</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>E32F1</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>As a user, I want to categorize customers by type (Prospect, Active, Key Account, Former)</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Create CCustomerType entity with workflow support. Initialize with default types: Prospect, Active Customer, Key Account, Strategic Partner, Former Customer.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>customers.customertype.domain.CCustomerType, customers.customertype.service.CCustomerTypeInitializerService</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>3</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>E32F1S3</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>E32F1</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>As a sales rep, I want to view and manage customers in a searchable grid with filters</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Create CCustomerInitializerService with grid view, detail section, sample data. Grid columns: name, type, status, industry, revenue, contact count, last interaction, assigned to. Create CCustomerService, CCustomerRepository, CPageServiceCustomer.</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>customers.customer.service.*</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>8</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>CRITICAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>E32F2S1</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>E32F2</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>As a sales rep, I want to manage contacts within customer accounts</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Create CContact entity: first name, last name, email, phone, mobile, title, department, isPrimary flag, linkedIn, preferredContactMethod, birthday, notes. ManyToOne with CCustomer. Implements IHasComments.</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>contacts.contact.domain.CContact</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>5</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>CRITICAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>E32F2S2</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>E32F2</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>As a user, I want to categorize contacts by role (Decision Maker, Influencer, User, etc.)</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Create CContactType entity. Initialize with default types: Decision Maker, Influencer, Technical Contact, End User, Champion, Blocker.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>contacts.contacttype.domain.CContactType</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>2</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>E32F2S3</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>E32F2</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>As a user, I want to view and search contacts with customer linkage</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Create CContactInitializerService with grid (columns: name, title, customer, email, phone, last contact date) and detail form. Create CContactService, CContactRepository, CPageServiceContact.</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>contacts.contact.service.*</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>8</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>E32F3S1</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>E32F3</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>As a marketing user, I want to capture and manage leads before they become customers</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Create CLead entity: company name, contact name, email, phone, lead source, lead score (0-100), status, qualification notes, assigned to user, estimated value, expected close date. Implements IHasStatusAndWorkflow, IHasComments.</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>leads.lead.domain.CLead</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>5</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>E32F3S2</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>E32F3</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>As a user, I want to track lead sources (Web, Referral, Event, Cold Call, etc.)</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Create CLeadSource entity. Initialize with default sources: Website, Referral, Trade Show, Cold Call, Email Campaign, Partner, Social Media, Advertisement.</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>leads.leadsource.domain.CLeadSource</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>2</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>E32F3S3</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>E32F3</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>As a sales manager, I want to view, qualify, and convert leads to opportunities</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Create CLeadInitializerService with grid (columns: company, contact, source, score, status, assigned to, expected value) and detail form. Add 'Convert to Opportunity' action button. Create CLeadService with convertToOpportunity() method.</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>leads.lead.service.*</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>8</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>E32F4S1</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>E32F4</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>As a sales rep, I want to track opportunities/deals with value and close date</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Create COpportunity entity: name, customer (ManyToOne), contact (ManyToOne), stage, probability (%), expected close date, amount, description, next steps, competition info. Implements IHasStatusAndWorkflow, IHasAttachments, IHasComments.</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>opportunities.opportunity.domain.COpportunity</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>5</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>CRITICAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>E32F4S2</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>E32F4</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>As a sales manager, I want to define pipeline stages (Qualification, Proposal, Negotiation, Closed Won/Lost)</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Create COpportunityStage entity with workflow. Initialize default stages: Lead, Qualification, Needs Analysis, Proposal, Negotiation, Closed Won, Closed Lost. Each stage has probability % and color.</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>opportunities.opportunitystage.domain.COpportunityStage</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>3</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>E32F4S3</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>E32F4</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>As a sales manager, I want to track win/loss reasons for closed opportunities</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Create CWinLossReason entity (isWinReason boolean). Initialize: Win reasons (Better Price, Better Product, Better Service), Loss reasons (Price, Competition, Timing, No Budget, Lost to Competitor).</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>opportunities.winlossreason.domain.CWinLossReason</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>2</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>E32F4S4</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>E32F4</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>As a user, I want to view opportunities in a pipeline board (Kanban-style) and grid</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Create COpportunityInitializerService with TWO views: (1) Standard grid+detail, (2) Pipeline board (Kanban). Grid columns: name, customer, stage, amount, probability, close date, assigned to. Pipeline board groups by stage with drag-drop. Create services and repositories.</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>opportunities.opportunity.service.*</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>13</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>CRITICAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>E32F5S1</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>E32F5</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>As a sales manager, I want to see a visual sales funnel with conversion rates</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Create CSalesFunnelComponent: Shows leads → opportunities → deals by stage. Displays count and value at each stage, conversion rates between stages. Uses Vaadin Charts.</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>pipeline.funnel.ui.CSalesFunnelComponent</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>8</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>E32F5S2</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>E32F5</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>As a sales manager, I want to view pipeline value by stage and time period</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Create CPipelineValueChart component: Bar/column chart showing total opportunity value by stage. Filter by date range, assigned user, customer segment. Create CPipelineAnalyticsService for data aggregation.</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>pipeline.dashboard.service.CPipelineAnalyticsService</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>5</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>E32F5S3</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>E32F5</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>As an executive, I want to see key CRM metrics dashboard (win rate, avg deal size, sales cycle)</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Create CCRMDashboard view: KPI cards (total customers, active opportunities, win rate %, avg deal size, avg sales cycle days). Charts: revenue by month, opportunities by stage, leads by source. Refresh button.</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>pipeline.dashboard.ui.CCRMDashboard</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>8</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>E32F6S1</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>E32F6</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>As a sales rep, I want to link activities and meetings to customers/contacts/opportunities</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Extend CActivity and CMeeting with optional references: customer (ManyToOne), contact (ManyToOne), opportunity (ManyToOne). Add activity type 'Customer Call', 'Customer Email', 'Demo', 'Follow-up'. Update initializers.</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>activities.activity.domain.CActivity</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>5</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>E32F6S2</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>E32F6</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>As a user, I want to see complete interaction history on customer detail page</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Add 'Interactions' tab to customer detail view showing related activities, meetings, comments, attachments ordered by date. Use CGrid with timeline visualization. Create CCustomerInteractionService.</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>customers.customer.service.CCustomerInteractionService</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>8</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
         </is>
       </c>
     </row>
@@ -17590,720 +18664,720 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" t="inlineStr">
+      <c r="A272" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B272" t="inlineStr">
+      <c r="B272" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C272" t="inlineStr">
+      <c r="C272" s="14" t="inlineStr">
         <is>
           <t>US13.3.2</t>
         </is>
       </c>
-      <c r="D272" t="inlineStr">
+      <c r="D272" s="14" t="inlineStr">
         <is>
           <t>Implement CComponentTestExecution - main execution interface</t>
         </is>
       </c>
-      <c r="E272" t="n">
+      <c r="E272" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F272" t="inlineStr">
+      <c r="F272" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G272" t="inlineStr">
+      <c r="G272" s="14" t="inlineStr">
         <is>
           <t>CComponentTestExecution.java</t>
         </is>
       </c>
-      <c r="H272" t="inlineStr">
+      <c r="H272" s="14" t="inlineStr">
         <is>
           <t>933 lines - Auto-save, keyboard shortcuts, ISO compliance - 2026-01-16</t>
         </is>
       </c>
     </row>
     <row r="273">
-      <c r="A273" t="inlineStr">
+      <c r="A273" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B273" t="inlineStr">
+      <c r="B273" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C273" t="inlineStr">
+      <c r="C273" s="14" t="inlineStr">
         <is>
           <t>US13.3.2</t>
         </is>
       </c>
-      <c r="D273" t="inlineStr">
+      <c r="D273" s="14" t="inlineStr">
         <is>
           <t>Update CPageServiceTestRun with component factory method</t>
         </is>
       </c>
-      <c r="E273" t="n">
+      <c r="E273" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F273" t="inlineStr">
+      <c r="F273" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G273" t="inlineStr">
+      <c r="G273" s="14" t="inlineStr">
         <is>
           <t>CPageServiceTestRun.java</t>
         </is>
       </c>
-      <c r="H273" t="inlineStr">
+      <c r="H273" s="14" t="inlineStr">
         <is>
           <t>createTestExecutionComponent() added - 2026-01-16</t>
         </is>
       </c>
     </row>
     <row r="274">
-      <c r="A274" t="inlineStr">
+      <c r="A274" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B274" t="inlineStr">
+      <c r="B274" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C274" t="inlineStr">
+      <c r="C274" s="14" t="inlineStr">
         <is>
           <t>US13.3.3</t>
         </is>
       </c>
-      <c r="D274" t="inlineStr">
+      <c r="D274" s="14" t="inlineStr">
         <is>
           <t>Add single-page execution view to CTestRunInitializerService</t>
         </is>
       </c>
-      <c r="E274" t="n">
+      <c r="E274" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F274" t="inlineStr">
+      <c r="F274" s="14" t="inlineStr">
         <is>
           <t>IN_PROGRESS</t>
         </is>
       </c>
-      <c r="G274" t="inlineStr">
+      <c r="G274" s="14" t="inlineStr">
         <is>
           <t>CTestRunInitializerService.java</t>
         </is>
       </c>
-      <c r="H274" t="inlineStr">
+      <c r="H274" s="14" t="inlineStr">
         <is>
           <t>Add second view with setAttributeNone(true) for full-screen execution</t>
         </is>
       </c>
     </row>
     <row r="275">
-      <c r="A275" t="inlineStr">
+      <c r="A275" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B275" t="inlineStr">
+      <c r="B275" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C275" t="inlineStr">
+      <c r="C275" s="14" t="inlineStr">
         <is>
           <t>US13.3.3</t>
         </is>
       </c>
-      <c r="D275" t="inlineStr">
+      <c r="D275" s="14" t="inlineStr">
         <is>
           <t>Add Execute button to test run detail view</t>
         </is>
       </c>
-      <c r="E275" t="n">
+      <c r="E275" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F275" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G275" t="inlineStr">
+      <c r="F275" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G275" s="14" t="inlineStr">
         <is>
           <t>Test run detail</t>
         </is>
       </c>
-      <c r="H275" t="inlineStr">
+      <c r="H275" s="14" t="inlineStr">
         <is>
           <t>Launch button for execution interface</t>
         </is>
       </c>
     </row>
     <row r="276">
-      <c r="A276" t="inlineStr">
+      <c r="A276" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B276" t="inlineStr">
+      <c r="B276" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C276" t="inlineStr">
+      <c r="C276" s="14" t="inlineStr">
         <is>
           <t>US13.3.4</t>
         </is>
       </c>
-      <c r="D276" t="inlineStr">
+      <c r="D276" s="14" t="inlineStr">
         <is>
           <t>Integrate screenshot capture functionality</t>
         </is>
       </c>
-      <c r="E276" t="n">
+      <c r="E276" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F276" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G276" t="inlineStr">
+      <c r="F276" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G276" s="14" t="inlineStr">
         <is>
           <t>CComponentTestExecution</t>
         </is>
       </c>
-      <c r="H276" t="inlineStr">
+      <c r="H276" s="14" t="inlineStr">
         <is>
           <t>Browser screenshot API for evidence</t>
         </is>
       </c>
     </row>
     <row r="277">
-      <c r="A277" t="inlineStr">
+      <c r="A277" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B277" t="inlineStr">
+      <c r="B277" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C277" t="inlineStr">
+      <c r="C277" s="14" t="inlineStr">
         <is>
           <t>US13.3.4</t>
         </is>
       </c>
-      <c r="D277" t="inlineStr">
+      <c r="D277" s="14" t="inlineStr">
         <is>
           <t>Implement file attachment upload in execution</t>
         </is>
       </c>
-      <c r="E277" t="n">
+      <c r="E277" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F277" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G277" t="inlineStr">
+      <c r="F277" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G277" s="14" t="inlineStr">
         <is>
           <t>CComponentTestExecution</t>
         </is>
       </c>
-      <c r="H277" t="inlineStr">
+      <c r="H277" s="14" t="inlineStr">
         <is>
           <t>Drag-drop file upload integration</t>
         </is>
       </c>
     </row>
     <row r="278">
-      <c r="A278" t="inlineStr">
+      <c r="A278" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B278" t="inlineStr">
+      <c r="B278" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C278" t="inlineStr">
+      <c r="C278" s="14" t="inlineStr">
         <is>
           <t>US13.1.4</t>
         </is>
       </c>
-      <c r="D278" t="inlineStr">
+      <c r="D278" s="14" t="inlineStr">
         <is>
           <t>Playwright: Test Cases CRUD operations</t>
         </is>
       </c>
-      <c r="E278" t="n">
+      <c r="E278" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F278" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G278" t="inlineStr">
+      <c r="F278" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G278" s="14" t="inlineStr">
         <is>
           <t>automated_tests/</t>
         </is>
       </c>
-      <c r="H278" t="inlineStr">
+      <c r="H278" s="14" t="inlineStr">
         <is>
           <t>Create, read, update, delete test cases</t>
         </is>
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="inlineStr">
+      <c r="A279" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B279" t="inlineStr">
+      <c r="B279" s="14" t="inlineStr">
         <is>
           <t>F13.2</t>
         </is>
       </c>
-      <c r="C279" t="inlineStr">
+      <c r="C279" s="14" t="inlineStr">
         <is>
           <t>US13.2.1</t>
         </is>
       </c>
-      <c r="D279" t="inlineStr">
+      <c r="D279" s="14" t="inlineStr">
         <is>
           <t>Playwright: Test Suites CRUD operations</t>
         </is>
       </c>
-      <c r="E279" t="n">
+      <c r="E279" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F279" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G279" t="inlineStr">
+      <c r="F279" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G279" s="14" t="inlineStr">
         <is>
           <t>automated_tests/</t>
         </is>
       </c>
-      <c r="H279" t="inlineStr">
+      <c r="H279" s="14" t="inlineStr">
         <is>
           <t>Create, read, update, delete test suites</t>
         </is>
       </c>
     </row>
     <row r="280">
-      <c r="A280" t="inlineStr">
+      <c r="A280" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B280" t="inlineStr">
+      <c r="B280" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C280" t="inlineStr">
+      <c r="C280" s="14" t="inlineStr">
         <is>
           <t>US13.3.1</t>
         </is>
       </c>
-      <c r="D280" t="inlineStr">
+      <c r="D280" s="14" t="inlineStr">
         <is>
           <t>Playwright: Test Session creation workflow</t>
         </is>
       </c>
-      <c r="E280" t="n">
+      <c r="E280" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F280" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G280" t="inlineStr">
+      <c r="F280" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G280" s="14" t="inlineStr">
         <is>
           <t>automated_tests/</t>
         </is>
       </c>
-      <c r="H280" t="inlineStr">
+      <c r="H280" s="14" t="inlineStr">
         <is>
           <t>Create session, link to suite</t>
         </is>
       </c>
     </row>
     <row r="281">
-      <c r="A281" t="inlineStr">
+      <c r="A281" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B281" t="inlineStr">
+      <c r="B281" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C281" t="inlineStr">
+      <c r="C281" s="14" t="inlineStr">
         <is>
           <t>US13.3.2</t>
         </is>
       </c>
-      <c r="D281" t="inlineStr">
+      <c r="D281" s="14" t="inlineStr">
         <is>
           <t>Playwright: Complete test execution workflow</t>
         </is>
       </c>
-      <c r="E281" t="n">
+      <c r="E281" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F281" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G281" t="inlineStr">
+      <c r="F281" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G281" s="14" t="inlineStr">
         <is>
           <t>automated_tests/</t>
         </is>
       </c>
-      <c r="H281" t="inlineStr">
+      <c r="H281" s="14" t="inlineStr">
         <is>
           <t>Execute test, record results, validate statistics</t>
         </is>
       </c>
     </row>
     <row r="282">
-      <c r="A282" t="inlineStr">
+      <c r="A282" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B282" t="inlineStr">
+      <c r="B282" s="14" t="inlineStr">
         <is>
           <t>F13.3</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
+      <c r="C282" s="14" t="inlineStr">
         <is>
           <t>US13.3.5</t>
         </is>
       </c>
-      <c r="D282" t="inlineStr">
+      <c r="D282" s="14" t="inlineStr">
         <is>
           <t>Playwright: Result recording validation</t>
         </is>
       </c>
-      <c r="E282" t="n">
+      <c r="E282" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F282" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G282" t="inlineStr">
+      <c r="F282" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G282" s="14" t="inlineStr">
         <is>
           <t>automated_tests/</t>
         </is>
       </c>
-      <c r="H282" t="inlineStr">
+      <c r="H282" s="14" t="inlineStr">
         <is>
           <t>Test PASS/FAIL/SKIP/BLOCK recording</t>
         </is>
       </c>
     </row>
     <row r="283">
-      <c r="A283" t="inlineStr">
+      <c r="A283" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B283" t="inlineStr">
+      <c r="B283" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C283" t="inlineStr">
+      <c r="C283" s="14" t="inlineStr">
         <is>
           <t>US13.5.1</t>
         </is>
       </c>
-      <c r="D283" t="inlineStr">
+      <c r="D283" s="14" t="inlineStr">
         <is>
           <t>Create test metrics dashboard component</t>
         </is>
       </c>
-      <c r="E283" t="n">
+      <c r="E283" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F283" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G283" t="inlineStr">
+      <c r="F283" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G283" s="14" t="inlineStr">
         <is>
           <t>CComponentTestMetrics</t>
         </is>
       </c>
-      <c r="H283" t="inlineStr">
+      <c r="H283" s="14" t="inlineStr">
         <is>
           <t>Charts: pass rate, coverage, trends</t>
         </is>
       </c>
     </row>
     <row r="284">
-      <c r="A284" t="inlineStr">
+      <c r="A284" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B284" t="inlineStr">
+      <c r="B284" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C284" t="inlineStr">
+      <c r="C284" s="14" t="inlineStr">
         <is>
           <t>US13.5.2</t>
         </is>
       </c>
-      <c r="D284" t="inlineStr">
+      <c r="D284" s="14" t="inlineStr">
         <is>
           <t>Implement test report generation service</t>
         </is>
       </c>
-      <c r="E284" t="n">
+      <c r="E284" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F284" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G284" t="inlineStr">
+      <c r="F284" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G284" s="14" t="inlineStr">
         <is>
           <t>CTestReportService</t>
         </is>
       </c>
-      <c r="H284" t="inlineStr">
+      <c r="H284" s="14" t="inlineStr">
         <is>
           <t>Export to PDF/Excel with charts</t>
         </is>
       </c>
     </row>
     <row r="285">
-      <c r="A285" t="inlineStr">
+      <c r="A285" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B285" t="inlineStr">
+      <c r="B285" s="14" t="inlineStr">
         <is>
           <t>F13.5</t>
         </is>
       </c>
-      <c r="C285" t="inlineStr">
+      <c r="C285" s="14" t="inlineStr">
         <is>
           <t>US13.5.3</t>
         </is>
       </c>
-      <c r="D285" t="inlineStr">
+      <c r="D285" s="14" t="inlineStr">
         <is>
           <t>Implement test coverage matrix by feature</t>
         </is>
       </c>
-      <c r="E285" t="n">
+      <c r="E285" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F285" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G285" t="inlineStr">
+      <c r="F285" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G285" s="14" t="inlineStr">
         <is>
           <t>CTestCoverageService</t>
         </is>
       </c>
-      <c r="H285" t="inlineStr">
+      <c r="H285" s="14" t="inlineStr">
         <is>
           <t>Link test cases to requirements</t>
         </is>
       </c>
     </row>
     <row r="286">
-      <c r="A286" t="inlineStr">
+      <c r="A286" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B286" t="inlineStr">
+      <c r="B286" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
+      <c r="C286" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D286" t="inlineStr">
+      <c r="D286" s="14" t="inlineStr">
         <is>
           <t>Run Spotless formatter on all test files</t>
         </is>
       </c>
-      <c r="E286" t="n">
+      <c r="E286" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F286" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G286" t="inlineStr">
+      <c r="F286" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G286" s="14" t="inlineStr">
         <is>
           <t>Maven spotless:apply</t>
         </is>
       </c>
-      <c r="H286" t="inlineStr">
+      <c r="H286" s="14" t="inlineStr">
         <is>
           <t>Format Java files to coding standards</t>
         </is>
       </c>
     </row>
     <row r="287">
-      <c r="A287" t="inlineStr">
+      <c r="A287" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B287" t="inlineStr">
+      <c r="B287" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C287" t="inlineStr">
+      <c r="C287" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D287" t="inlineStr">
+      <c r="D287" s="14" t="inlineStr">
         <is>
           <t>Run CodeQL security scan</t>
         </is>
       </c>
-      <c r="E287" t="n">
+      <c r="E287" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F287" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G287" t="inlineStr">
+      <c r="F287" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G287" s="14" t="inlineStr">
         <is>
           <t>GitHub Actions</t>
         </is>
       </c>
-      <c r="H287" t="inlineStr">
+      <c r="H287" s="14" t="inlineStr">
         <is>
           <t>Security vulnerability check</t>
         </is>
       </c>
     </row>
     <row r="288">
-      <c r="A288" t="inlineStr">
+      <c r="A288" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B288" t="inlineStr">
+      <c r="B288" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C288" t="inlineStr">
+      <c r="C288" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D288" t="inlineStr">
+      <c r="D288" s="14" t="inlineStr">
         <is>
           <t>Update terminology with ISO/ISTQB UI standards</t>
         </is>
       </c>
-      <c r="E288" t="n">
+      <c r="E288" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F288" t="inlineStr">
+      <c r="F288" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G288" t="inlineStr">
+      <c r="G288" s="14" t="inlineStr">
         <is>
           <t>TESTING_TERMINOLOGY_MAPPING.md</t>
         </is>
       </c>
-      <c r="H288" t="inlineStr">
+      <c r="H288" s="14" t="inlineStr">
         <is>
           <t>UI component standards added - 2026-01-16</t>
         </is>
       </c>
     </row>
     <row r="289">
-      <c r="A289" t="inlineStr">
+      <c r="A289" s="14" t="inlineStr">
         <is>
           <t>E13</t>
         </is>
       </c>
-      <c r="B289" t="inlineStr">
+      <c r="B289" s="14" t="inlineStr">
         <is>
           <t>F13.1</t>
         </is>
       </c>
-      <c r="C289" t="inlineStr">
+      <c r="C289" s="14" t="inlineStr">
         <is>
           <t>US13.1.1</t>
         </is>
       </c>
-      <c r="D289" t="inlineStr">
+      <c r="D289" s="14" t="inlineStr">
         <is>
           <t>Create code pattern compliance audit</t>
         </is>
       </c>
-      <c r="E289" t="n">
+      <c r="E289" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F289" t="inlineStr">
+      <c r="F289" s="14" t="inlineStr">
         <is>
           <t>DONE</t>
         </is>
       </c>
-      <c r="G289" t="inlineStr">
+      <c r="G289" s="14" t="inlineStr">
         <is>
           <t>CODE_PATTERN_COMPLIANCE_AUDIT.md</t>
         </is>
       </c>
-      <c r="H289" t="inlineStr">
+      <c r="H289" s="14" t="inlineStr">
         <is>
           <t>100% pattern compliance verified - 2026-01-16</t>
         </is>

</xml_diff>

<commit_message>
Add storage inventory backlog entries
Co-authored-by: yalovali <234063+yalovali@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/__PROJECT_BACKLOG.xlsx
+++ b/docs/__PROJECT_BACKLOG.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
@@ -2176,66 +2176,126 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="14" t="inlineStr">
         <is>
           <t>E32</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="14" t="inlineStr">
         <is>
           <t>CRM &amp; Customer Relationship Management</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="14" t="inlineStr">
         <is>
           <t>Complete CRM system with customer/account management, contact tracking, lead management, opportunity/deal pipeline, sales funnel visualization, customer interactions, and customer analytics. Enables comprehensive customer lifecycle management.</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="14" t="inlineStr">
         <is>
           <t>Enables customer-centric operations, improves sales pipeline visibility, tracks customer interactions, forecasts revenue, manages customer lifecycle, supports sales team efficiency, provides customer insights and analytics.</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
+      <c r="E33" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F33" s="14" t="inlineStr">
         <is>
           <t>Not Implemented</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G33" s="14" t="inlineStr">
         <is>
           <t>customers, contacts, leads, opportunities, deals, salespipeline</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="H33" s="14" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="I33" s="14" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="J33" s="14" t="inlineStr">
         <is>
           <t>54</t>
         </is>
       </c>
-      <c r="K33">
+      <c r="K33" s="14">
         <f>SUMIF(Features!B:B,A33,Features!I:I)</f>
         <v/>
       </c>
-      <c r="L33" t="inlineStr">
+      <c r="L33" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr">
+      <c r="M33" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>E33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Storage &amp; Inventory Management</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Enterprise storage hierarchy, inventory items with counts, audit-trailed stock transactions, low-stock/expiration alerts, and supplier-aware restocking.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Prevents stockouts and overstock, increases visibility of consumables, enables auditability of stock movements, and centralizes warehouse operations across multiple locations.</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>PLANNED</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>CStorage, CStorageItem, CStorageTransaction, CStorageType, CStorageItemType, CTransactionType</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>plm.storage (planned)</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>4</v>
+      </c>
+      <c r="I34" t="n">
+        <v>13</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f>SUMIF(Features!B:B,A34,Features!I:I)</f>
+        <v/>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
@@ -2255,7 +2315,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
@@ -4183,303 +4243,526 @@
       </c>
     </row>
     <row r="38" ht="13.5" customHeight="1" s="15">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="14" t="inlineStr">
         <is>
           <t>E32F1</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="14" t="inlineStr">
         <is>
           <t>E32</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="14" t="inlineStr">
         <is>
           <t>Customer &amp; Account Management</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="14" t="inlineStr">
         <is>
           <t>Comprehensive customer/account entity with company details, industry classification, relationship type, customer status, revenue tracking, and customer lifecycle management.</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E38" s="14" t="inlineStr">
         <is>
           <t>Centralizes customer data, tracks customer health, manages customer hierarchy, supports account-based selling.</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
+      <c r="F38" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G38" s="14" t="inlineStr">
         <is>
           <t>customers.customer, customers.customertype</t>
         </is>
       </c>
-      <c r="H38" t="n">
+      <c r="H38" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="14">
         <f>SUMIF(User_Stories!B:B,A38,User_Stories!H:H)</f>
         <v/>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="J38" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="39" ht="13.5" customHeight="1" s="15">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="14" t="inlineStr">
         <is>
           <t>E32F2</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="14" t="inlineStr">
         <is>
           <t>E32</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="14" t="inlineStr">
         <is>
           <t>Contact Management</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="14" t="inlineStr">
         <is>
           <t>Individual contact records linked to customers with full contact details, role/title tracking, communication preferences, interaction history, and relationship strength scoring.</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E39" s="14" t="inlineStr">
         <is>
           <t>Enables person-level relationship tracking, manages contact hierarchies, tracks communication preferences, improves outreach effectiveness.</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
+      <c r="F39" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G39" s="14" t="inlineStr">
         <is>
           <t>contacts.contact, contacts.contacttype</t>
         </is>
       </c>
-      <c r="H39" t="n">
+      <c r="H39" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="14">
         <f>SUMIF(User_Stories!B:B,A39,User_Stories!H:H)</f>
         <v/>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="J39" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="40" ht="13.5" customHeight="1" s="15">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="14" t="inlineStr">
         <is>
           <t>E32F3</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="14" t="inlineStr">
         <is>
           <t>E32</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="14" t="inlineStr">
         <is>
           <t>Lead Management &amp; Qualification</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="14" t="inlineStr">
         <is>
           <t>Lead capture, scoring, qualification, and conversion tracking. Manages leads from first contact through qualification to opportunity conversion.</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E40" s="14" t="inlineStr">
         <is>
           <t>Captures early-stage prospects, prioritizes leads by score, tracks lead sources, measures conversion rates, prevents lead leakage.</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
+      <c r="F40" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G40" s="14" t="inlineStr">
         <is>
           <t>leads.lead, leads.leadsource, leads.leadstatus</t>
         </is>
       </c>
-      <c r="H40" t="n">
+      <c r="H40" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="14">
         <f>SUMIF(User_Stories!B:B,A40,User_Stories!H:H)</f>
         <v/>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="J40" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="41" ht="13.5" customHeight="1" s="15">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="14" t="inlineStr">
         <is>
           <t>E32F4</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="14" t="inlineStr">
         <is>
           <t>E32</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="14" t="inlineStr">
         <is>
           <t>Opportunity &amp; Deal Pipeline Management</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="14" t="inlineStr">
         <is>
           <t>Sales opportunity tracking with pipeline stages, probability tracking, expected close dates, deal value, competitive tracking, and win/loss analysis.</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E41" s="14" t="inlineStr">
         <is>
           <t>Visualizes sales pipeline, forecasts revenue, tracks deal progress, identifies bottlenecks, improves win rates through analysis.</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
+      <c r="F41" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G41" s="14" t="inlineStr">
         <is>
           <t>opportunities.opportunity, opportunities.opportunitystage, opportunities.winlossreason</t>
         </is>
       </c>
-      <c r="H41" t="n">
+      <c r="H41" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="14">
         <f>SUMIF(User_Stories!B:B,A41,User_Stories!H:H)</f>
         <v/>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="J41" s="14" t="inlineStr">
         <is>
           <t>CRITICAL</t>
         </is>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1" s="15">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="14" t="inlineStr">
         <is>
           <t>E32F5</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="14" t="inlineStr">
         <is>
           <t>E32</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="14" t="inlineStr">
         <is>
           <t>Sales Funnel &amp; Pipeline Analytics</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="14" t="inlineStr">
         <is>
           <t>Visual sales funnel showing conversion rates between stages, pipeline value analysis, forecast accuracy tracking, and sales velocity metrics.</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E42" s="14" t="inlineStr">
         <is>
           <t>Identifies pipeline bottlenecks, forecasts revenue accurately, measures sales efficiency, tracks conversion rates, supports data-driven sales decisions.</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
+      <c r="F42" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G42" s="14" t="inlineStr">
         <is>
           <t>pipeline.dashboard, pipeline.funnel</t>
         </is>
       </c>
-      <c r="H42" t="n">
+      <c r="H42" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="14">
         <f>SUMIF(User_Stories!B:B,A42,User_Stories!H:H)</f>
         <v/>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="J42" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="43" ht="13.5" customHeight="1" s="15">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="14" t="inlineStr">
         <is>
           <t>E32F6</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="14" t="inlineStr">
         <is>
           <t>E32</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="14" t="inlineStr">
         <is>
           <t>Customer Interaction &amp; Activity Tracking</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="14" t="inlineStr">
         <is>
           <t>Log and track all customer touchpoints including calls, emails, meetings, demos, and custom activities. Maintains complete interaction history per customer.</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E43" s="14" t="inlineStr">
         <is>
           <t>Provides 360° customer view, improves handoffs, tracks engagement frequency, ensures follow-up, supports relationship quality scoring.</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
+      <c r="F43" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G43" s="14" t="inlineStr">
         <is>
           <t>Leverage existing CActivity and CMeeting</t>
         </is>
       </c>
-      <c r="H43" t="n">
+      <c r="H43" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="14">
         <f>SUMIF(User_Stories!B:B,A43,User_Stories!H:H)</f>
         <v/>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="J43" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
     </row>
-    <row r="44" ht="13.5" customHeight="1" s="15"/>
-    <row r="45" ht="13.5" customHeight="1" s="15"/>
-    <row r="46" ht="13.5" customHeight="1" s="15"/>
-    <row r="47" ht="13.5" customHeight="1" s="15"/>
+    <row r="44" ht="13.5" customHeight="1" s="15">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>E33F1</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>E33</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Storage Location Hierarchy &amp; Capacity</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Manage multi-level storage locations with types, parent-child hierarchy, capacity, environment, and responsible ownership.</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>✓ Create storage locations with parent-child hierarchy
+✓ Define storage types (warehouse, room, shelf)
+✓ Track capacity/utilization and environment controls
+✓ Assign responsible user and active flag</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Implement CStorage entity/service with parentStorage reference, capacity/utilization helpers, and location path rendering.</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>CStorage, CStorageType, CStorageService, CStorageInitializerService</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <f>SUMIF(User_Stories!B:B,A44,User_Stories!F:F)</f>
+        <v/>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="13.5" customHeight="1" s="15">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>E33F2</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>E33</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Inventory Item Definition &amp; Compliance</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Define storage items with SKU/barcode, type, stock thresholds, supplier data, expiration handling, and special handling rules.</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>✓ Create storage items with SKU/barcode and type
+✓ Capture stock thresholds (min/max/reorder) and unit of measure
+✓ Track supplier, lead time, and special handling/expiration data</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Define CStorageItem with quantity, thresholds, supplier link, and expiration fields; service validates SKU/barcode uniqueness and unit conversions.</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>CStorageItem, CStorageItemType, CStorageItemService, CStorageItemInitializerService</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>3</v>
+      </c>
+      <c r="I45">
+        <f>SUMIF(User_Stories!B:B,A45,User_Stories!F:F)</f>
+        <v/>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" ht="13.5" customHeight="1" s="15">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>E33F3</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>E33</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Stock Operations &amp; Transaction Audit Trail</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Provide stock intake, issuance, adjustment, and transfer with immutable transaction history for every movement.</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>✓ Add/remove stock with validation and auto transaction log
+✓ Adjust stock with before/after quantities and reasons
+✓ Transfer stock between locations with dual transactions
+✓ Support transaction types for expired/damaged/lost</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Provide addStock/removeStock/adjustStock/transferStock methods in CStorageItemService and persist immutable CStorageTransaction entries (comment-style records).</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>CStorageTransaction, CTransactionType, CStorageTransactionService, CStorageItemService</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <f>SUMIF(User_Stories!B:B,A46,User_Stories!F:F)</f>
+        <v/>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="13.5" customHeight="1" s="15">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>E33F4</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>E33</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Alerts &amp; Reporting for Storage</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Deliver operational visibility with low-stock and expiration alerts plus transaction history and value/utilization summaries.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>✓ Low-stock alerts based on minimum levels
+✓ Expiration monitoring with expiring-soon threshold
+✓ Transaction history grids with filters
+✓ Stock value and utilization summaries</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Query helpers getLowStockItems/getExpiredItems/getItemsExpiringSoon plus history views using grid column helpers.</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>CStorageItemService, CStorageTransactionService</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <f>SUMIF(User_Stories!B:B,A47,User_Stories!F:F)</f>
+        <v/>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
     <row r="48" ht="13.5" customHeight="1" s="15"/>
     <row r="49" ht="13.5" customHeight="1" s="15"/>
   </sheetData>
@@ -4496,7 +4779,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
@@ -7026,722 +7309,1242 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="14" t="inlineStr">
         <is>
           <t>E32F1S1</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B66" s="14" t="inlineStr">
         <is>
           <t>E32F1</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C66" s="14" t="inlineStr">
         <is>
           <t>As a sales manager, I want to create and manage customer accounts with detailed company information</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="D66" s="14" t="inlineStr">
         <is>
           <t>Create CCustomer entity with fields: company name, industry, size, website, revenue, customer type, status, relationship start date, description, logo. Extends CProjectItem. Implements IHasStatusAndWorkflow, IHasAttachments, IHasComments.</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
+      <c r="E66" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F66" s="14" t="inlineStr">
         <is>
           <t>customers.customer.domain.CCustomer</t>
         </is>
       </c>
-      <c r="G66" t="n">
+      <c r="G66" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="H66" t="inlineStr">
+      <c r="H66" s="14" t="inlineStr">
         <is>
           <t>CRITICAL</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="14" t="inlineStr">
         <is>
           <t>E32F1S2</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B67" s="14" t="inlineStr">
         <is>
           <t>E32F1</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C67" s="14" t="inlineStr">
         <is>
           <t>As a user, I want to categorize customers by type (Prospect, Active, Key Account, Former)</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="D67" s="14" t="inlineStr">
         <is>
           <t>Create CCustomerType entity with workflow support. Initialize with default types: Prospect, Active Customer, Key Account, Strategic Partner, Former Customer.</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
+      <c r="E67" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F67" s="14" t="inlineStr">
         <is>
           <t>customers.customertype.domain.CCustomerType, customers.customertype.service.CCustomerTypeInitializerService</t>
         </is>
       </c>
-      <c r="G67" t="n">
+      <c r="G67" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="H67" t="inlineStr">
+      <c r="H67" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" s="14" t="inlineStr">
         <is>
           <t>E32F1S3</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B68" s="14" t="inlineStr">
         <is>
           <t>E32F1</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C68" s="14" t="inlineStr">
         <is>
           <t>As a sales rep, I want to view and manage customers in a searchable grid with filters</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D68" s="14" t="inlineStr">
         <is>
           <t>Create CCustomerInitializerService with grid view, detail section, sample data. Grid columns: name, type, status, industry, revenue, contact count, last interaction, assigned to. Create CCustomerService, CCustomerRepository, CPageServiceCustomer.</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
+      <c r="E68" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F68" s="14" t="inlineStr">
         <is>
           <t>customers.customer.service.*</t>
         </is>
       </c>
-      <c r="G68" t="n">
+      <c r="G68" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="H68" t="inlineStr">
+      <c r="H68" s="14" t="inlineStr">
         <is>
           <t>CRITICAL</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="14" t="inlineStr">
         <is>
           <t>E32F2S1</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B69" s="14" t="inlineStr">
         <is>
           <t>E32F2</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C69" s="14" t="inlineStr">
         <is>
           <t>As a sales rep, I want to manage contacts within customer accounts</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="D69" s="14" t="inlineStr">
         <is>
           <t>Create CContact entity: first name, last name, email, phone, mobile, title, department, isPrimary flag, linkedIn, preferredContactMethod, birthday, notes. ManyToOne with CCustomer. Implements IHasComments.</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
+      <c r="E69" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F69" s="14" t="inlineStr">
         <is>
           <t>contacts.contact.domain.CContact</t>
         </is>
       </c>
-      <c r="G69" t="n">
+      <c r="G69" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="H69" t="inlineStr">
+      <c r="H69" s="14" t="inlineStr">
         <is>
           <t>CRITICAL</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="14" t="inlineStr">
         <is>
           <t>E32F2S2</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B70" s="14" t="inlineStr">
         <is>
           <t>E32F2</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C70" s="14" t="inlineStr">
         <is>
           <t>As a user, I want to categorize contacts by role (Decision Maker, Influencer, User, etc.)</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="D70" s="14" t="inlineStr">
         <is>
           <t>Create CContactType entity. Initialize with default types: Decision Maker, Influencer, Technical Contact, End User, Champion, Blocker.</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
+      <c r="E70" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F70" s="14" t="inlineStr">
         <is>
           <t>contacts.contacttype.domain.CContactType</t>
         </is>
       </c>
-      <c r="G70" t="n">
+      <c r="G70" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="H70" t="inlineStr">
+      <c r="H70" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="14" t="inlineStr">
         <is>
           <t>E32F2S3</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B71" s="14" t="inlineStr">
         <is>
           <t>E32F2</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C71" s="14" t="inlineStr">
         <is>
           <t>As a user, I want to view and search contacts with customer linkage</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D71" s="14" t="inlineStr">
         <is>
           <t>Create CContactInitializerService with grid (columns: name, title, customer, email, phone, last contact date) and detail form. Create CContactService, CContactRepository, CPageServiceContact.</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
+      <c r="E71" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F71" s="14" t="inlineStr">
         <is>
           <t>contacts.contact.service.*</t>
         </is>
       </c>
-      <c r="G71" t="n">
+      <c r="G71" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="H71" t="inlineStr">
+      <c r="H71" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
+      <c r="A72" s="14" t="inlineStr">
         <is>
           <t>E32F3S1</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B72" s="14" t="inlineStr">
         <is>
           <t>E32F3</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C72" s="14" t="inlineStr">
         <is>
           <t>As a marketing user, I want to capture and manage leads before they become customers</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="D72" s="14" t="inlineStr">
         <is>
           <t>Create CLead entity: company name, contact name, email, phone, lead source, lead score (0-100), status, qualification notes, assigned to user, estimated value, expected close date. Implements IHasStatusAndWorkflow, IHasComments.</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
+      <c r="E72" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F72" s="14" t="inlineStr">
         <is>
           <t>leads.lead.domain.CLead</t>
         </is>
       </c>
-      <c r="G72" t="n">
+      <c r="G72" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="H72" t="inlineStr">
+      <c r="H72" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" s="14" t="inlineStr">
         <is>
           <t>E32F3S2</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B73" s="14" t="inlineStr">
         <is>
           <t>E32F3</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C73" s="14" t="inlineStr">
         <is>
           <t>As a user, I want to track lead sources (Web, Referral, Event, Cold Call, etc.)</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D73" s="14" t="inlineStr">
         <is>
           <t>Create CLeadSource entity. Initialize with default sources: Website, Referral, Trade Show, Cold Call, Email Campaign, Partner, Social Media, Advertisement.</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
+      <c r="E73" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F73" s="14" t="inlineStr">
         <is>
           <t>leads.leadsource.domain.CLeadSource</t>
         </is>
       </c>
-      <c r="G73" t="n">
+      <c r="G73" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="H73" t="inlineStr">
+      <c r="H73" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" s="14" t="inlineStr">
         <is>
           <t>E32F3S3</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B74" s="14" t="inlineStr">
         <is>
           <t>E32F3</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C74" s="14" t="inlineStr">
         <is>
           <t>As a sales manager, I want to view, qualify, and convert leads to opportunities</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="D74" s="14" t="inlineStr">
         <is>
           <t>Create CLeadInitializerService with grid (columns: company, contact, source, score, status, assigned to, expected value) and detail form. Add 'Convert to Opportunity' action button. Create CLeadService with convertToOpportunity() method.</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
+      <c r="E74" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F74" s="14" t="inlineStr">
         <is>
           <t>leads.lead.service.*</t>
         </is>
       </c>
-      <c r="G74" t="n">
+      <c r="G74" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="H74" t="inlineStr">
+      <c r="H74" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="A75" s="14" t="inlineStr">
         <is>
           <t>E32F4S1</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B75" s="14" t="inlineStr">
         <is>
           <t>E32F4</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C75" s="14" t="inlineStr">
         <is>
           <t>As a sales rep, I want to track opportunities/deals with value and close date</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="D75" s="14" t="inlineStr">
         <is>
           <t>Create COpportunity entity: name, customer (ManyToOne), contact (ManyToOne), stage, probability (%), expected close date, amount, description, next steps, competition info. Implements IHasStatusAndWorkflow, IHasAttachments, IHasComments.</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
+      <c r="E75" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F75" s="14" t="inlineStr">
         <is>
           <t>opportunities.opportunity.domain.COpportunity</t>
         </is>
       </c>
-      <c r="G75" t="n">
+      <c r="G75" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="H75" t="inlineStr">
+      <c r="H75" s="14" t="inlineStr">
         <is>
           <t>CRITICAL</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
+      <c r="A76" s="14" t="inlineStr">
         <is>
           <t>E32F4S2</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B76" s="14" t="inlineStr">
         <is>
           <t>E32F4</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C76" s="14" t="inlineStr">
         <is>
           <t>As a sales manager, I want to define pipeline stages (Qualification, Proposal, Negotiation, Closed Won/Lost)</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="D76" s="14" t="inlineStr">
         <is>
           <t>Create COpportunityStage entity with workflow. Initialize default stages: Lead, Qualification, Needs Analysis, Proposal, Negotiation, Closed Won, Closed Lost. Each stage has probability % and color.</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
+      <c r="E76" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F76" s="14" t="inlineStr">
         <is>
           <t>opportunities.opportunitystage.domain.COpportunityStage</t>
         </is>
       </c>
-      <c r="G76" t="n">
+      <c r="G76" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="H76" t="inlineStr">
+      <c r="H76" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
+      <c r="A77" s="14" t="inlineStr">
         <is>
           <t>E32F4S3</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B77" s="14" t="inlineStr">
         <is>
           <t>E32F4</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C77" s="14" t="inlineStr">
         <is>
           <t>As a sales manager, I want to track win/loss reasons for closed opportunities</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="D77" s="14" t="inlineStr">
         <is>
           <t>Create CWinLossReason entity (isWinReason boolean). Initialize: Win reasons (Better Price, Better Product, Better Service), Loss reasons (Price, Competition, Timing, No Budget, Lost to Competitor).</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
+      <c r="E77" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F77" s="14" t="inlineStr">
         <is>
           <t>opportunities.winlossreason.domain.CWinLossReason</t>
         </is>
       </c>
-      <c r="G77" t="n">
+      <c r="G77" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="H77" t="inlineStr">
+      <c r="H77" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" s="14" t="inlineStr">
         <is>
           <t>E32F4S4</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B78" s="14" t="inlineStr">
         <is>
           <t>E32F4</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C78" s="14" t="inlineStr">
         <is>
           <t>As a user, I want to view opportunities in a pipeline board (Kanban-style) and grid</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="D78" s="14" t="inlineStr">
         <is>
           <t>Create COpportunityInitializerService with TWO views: (1) Standard grid+detail, (2) Pipeline board (Kanban). Grid columns: name, customer, stage, amount, probability, close date, assigned to. Pipeline board groups by stage with drag-drop. Create services and repositories.</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
+      <c r="E78" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F78" s="14" t="inlineStr">
         <is>
           <t>opportunities.opportunity.service.*</t>
         </is>
       </c>
-      <c r="G78" t="n">
+      <c r="G78" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="H78" t="inlineStr">
+      <c r="H78" s="14" t="inlineStr">
         <is>
           <t>CRITICAL</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
+      <c r="A79" s="14" t="inlineStr">
         <is>
           <t>E32F5S1</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B79" s="14" t="inlineStr">
         <is>
           <t>E32F5</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C79" s="14" t="inlineStr">
         <is>
           <t>As a sales manager, I want to see a visual sales funnel with conversion rates</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="D79" s="14" t="inlineStr">
         <is>
           <t>Create CSalesFunnelComponent: Shows leads → opportunities → deals by stage. Displays count and value at each stage, conversion rates between stages. Uses Vaadin Charts.</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
+      <c r="E79" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F79" s="14" t="inlineStr">
         <is>
           <t>pipeline.funnel.ui.CSalesFunnelComponent</t>
         </is>
       </c>
-      <c r="G79" t="n">
+      <c r="G79" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="H79" t="inlineStr">
+      <c r="H79" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
+      <c r="A80" s="14" t="inlineStr">
         <is>
           <t>E32F5S2</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="B80" s="14" t="inlineStr">
         <is>
           <t>E32F5</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="C80" s="14" t="inlineStr">
         <is>
           <t>As a sales manager, I want to view pipeline value by stage and time period</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
+      <c r="D80" s="14" t="inlineStr">
         <is>
           <t>Create CPipelineValueChart component: Bar/column chart showing total opportunity value by stage. Filter by date range, assigned user, customer segment. Create CPipelineAnalyticsService for data aggregation.</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
+      <c r="E80" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F80" s="14" t="inlineStr">
         <is>
           <t>pipeline.dashboard.service.CPipelineAnalyticsService</t>
         </is>
       </c>
-      <c r="G80" t="n">
+      <c r="G80" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="H80" t="inlineStr">
+      <c r="H80" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
+      <c r="A81" s="14" t="inlineStr">
         <is>
           <t>E32F5S3</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B81" s="14" t="inlineStr">
         <is>
           <t>E32F5</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C81" s="14" t="inlineStr">
         <is>
           <t>As an executive, I want to see key CRM metrics dashboard (win rate, avg deal size, sales cycle)</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="D81" s="14" t="inlineStr">
         <is>
           <t>Create CCRMDashboard view: KPI cards (total customers, active opportunities, win rate %, avg deal size, avg sales cycle days). Charts: revenue by month, opportunities by stage, leads by source. Refresh button.</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
+      <c r="E81" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F81" s="14" t="inlineStr">
         <is>
           <t>pipeline.dashboard.ui.CCRMDashboard</t>
         </is>
       </c>
-      <c r="G81" t="n">
+      <c r="G81" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="H81" t="inlineStr">
+      <c r="H81" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
+      <c r="A82" s="14" t="inlineStr">
         <is>
           <t>E32F6S1</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B82" s="14" t="inlineStr">
         <is>
           <t>E32F6</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="C82" s="14" t="inlineStr">
         <is>
           <t>As a sales rep, I want to link activities and meetings to customers/contacts/opportunities</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="D82" s="14" t="inlineStr">
         <is>
           <t>Extend CActivity and CMeeting with optional references: customer (ManyToOne), contact (ManyToOne), opportunity (ManyToOne). Add activity type 'Customer Call', 'Customer Email', 'Demo', 'Follow-up'. Update initializers.</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
+      <c r="E82" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F82" s="14" t="inlineStr">
         <is>
           <t>activities.activity.domain.CActivity</t>
         </is>
       </c>
-      <c r="G82" t="n">
+      <c r="G82" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="H82" t="inlineStr">
+      <c r="H82" s="14" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
+      <c r="A83" s="14" t="inlineStr">
         <is>
           <t>E32F6S2</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B83" s="14" t="inlineStr">
         <is>
           <t>E32F6</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="C83" s="14" t="inlineStr">
         <is>
           <t>As a user, I want to see complete interaction history on customer detail page</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
+      <c r="D83" s="14" t="inlineStr">
         <is>
           <t>Add 'Interactions' tab to customer detail view showing related activities, meetings, comments, attachments ordered by date. Use CGrid with timeline visualization. Create CCustomerInteractionService.</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
+      <c r="E83" s="14" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F83" s="14" t="inlineStr">
         <is>
           <t>customers.customer.service.CCustomerInteractionService</t>
         </is>
       </c>
-      <c r="G83" t="n">
+      <c r="G83" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="H83" t="inlineStr">
+      <c r="H83" s="14" t="inlineStr">
         <is>
           <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>E33F1S1</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>E33F1</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>As a warehouse manager, I can create hierarchical storage locations with types</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Given a project, when I add a storage location, then I can select a parent (warehouse/room/shelf), choose a storage type, and see the full location path.</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>CStorage extends CProjectItem with parentStorage self-reference and getLocationPath(); CStorageType combo via CStorageTypeService.</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>5</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>E33F1S2</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>E33F1</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>As a staff member, I can capture capacity, utilization, and environment settings for a storage location</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Given a storage location, when I edit details, then I can set capacity/unit, current utilization, temperature/climate controls, secure storage flag, and responsible user.</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Fields: capacity, capacityUnit, currentUtilization, temperatureControl, climateControl, secureStorage, responsibleUser; getUtilizationPercentage() helper.</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>5</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>E33F1S3</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>E33F1</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>As an admin, I cannot delete a storage location that still has child locations or items</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Given a storage with children or assigned items, when I attempt deletion, then the system blocks it with a validation message.</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>CStorageService.checkDeleteAllowed() validates parent/child hierarchy and linked CStorageItem records.</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>3</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>E33F2S1</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>E33F2</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>As a warehouse manager, I can create storage items with SKU and barcode linked to a storage location</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Given a storage location, when I add an item, then I set name, type, SKU, barcode, and storage reference; duplicate SKU/barcode in the same project are rejected.</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>CStorageItem extends CProjectItem with storage reference; validateEntity enforces project-scoped SKU/barcode uniqueness; FormBuilder shows SKU/barcode fields.</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>5</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>E33F2S2</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>E33F2</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>As a purchasing manager, I can maintain stock thresholds and reorder settings</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Given a storage item, when I edit thresholds, then I can set unit of measure, minimum stock level, reorder quantity, and maximum stock level to drive alerts.</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>CStorageItem numeric fields with validation feed isLowStock() and getStockPercentage(); reorderQuantity used for purchase suggestions.</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>5</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>E33F2S3</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>E33F2</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>As a quality manager, I can track batches, expiration, and special handling requirements</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Given an item with expiration tracking enabled, when I save details, then batch number and expiration date are stored and special handling instructions are captured.</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>trackExpiration flag controls isExpired()/isExpiringSoon(); handlingInstructions text with max length; requiresSpecialHandling boolean.</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>3</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>E33F3S1</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>E33F3</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>As a warehouse worker, I can receive stock with an audit trail</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Given a storage item, when I record incoming quantity, then the system increases current quantity and creates a STOCK_IN transaction capturing before/after, user, timestamp, and description.</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>CStorageItemService.addStock() wraps save and CStorageTransactionService.createTransaction(CTransactionType.STOCK_IN); updates lastRestockedDate.</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>5</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>E33F3S2</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>E33F3</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>As a staff member, I can issue or remove stock with validation</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Given available stock, when I issue quantity for consumption, then removeStock validates availability, decrements quantity, and logs STOCK_OUT/DAMAGED/LOST/EXPIRED transaction with reason.</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>removeStock() prevents negative quantities; description stored like comment note; transaction type parameterized.</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>5</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>E33F3S3</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>E33F3</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>As an auditor, I can adjust stock counts while preserving an immutable trail</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Given a discrepancy, when I adjust to a new quantity, then the system records an ADJUSTMENT transaction with before/after values and required reason while existing transactions remain unchanged.</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>adjustStock() captures quantityBefore/After and description; CStorageTransaction records are immutable (no updates/deletes).</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>3</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>E33F3S4</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>E33F3</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>As a warehouse worker, I can transfer stock between storage locations</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Given a source and target item, when I transfer quantity, then the system validates source stock, decrements source, increments target, and records paired TRANSFER transactions with shared description/reference.</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>transferStock() creates OUT and IN CStorageTransaction entries using CTransactionType.TRANSFER; enforces same SKU when linking source/target.</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>5</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>E33F4S1</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>E33F4</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>As a purchasing manager, I can view low-stock items ready for reorder</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Given minimum stock levels, when I view storage alerts, then I see items where current quantity is at or below minimum, sorted by quantity.</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>CStorageItemService.getLowStockItems(project) query with ORDER BY; grid shows unitOfMeasure and reorderQuantity.</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>3</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>E33F4S2</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>E33F4</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>As a staff member, I can monitor expired and expiring items</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Given items with expiration tracking, when I open the expiration view, then I see expired items and items expiring within a configurable number of days.</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>getExpiredItems() and getItemsExpiringSoon(project, days) use LocalDate filters; include batchNumber and expirationDate columns.</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>3</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>E33F4S3</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>E33F4</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>As an auditor, I can review full transaction history for a storage item</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Given a storage item, when I open its history, then I can filter by transaction type or date range and see before/after quantities, user, and descriptions.</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>CStorageTransactionService.getTransactionsForItem(), getTransactionsByType(), getTransactionsByDateRange(); grid uses entity column helpers; transactions act like comment-style records.</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>5</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>TODO</t>
         </is>
       </c>
     </row>

</xml_diff>